<commit_message>
bug fixes, adjusted data-set size
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbalkovec/Desktop/CPSC4100/FinalProject/FinalProject4100/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBF21EAE-11DF-7E4D-B1BB-1204393DFAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9329C6D2-5355-A84C-B22F-CD430B65BD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="500" windowWidth="27200" windowHeight="16940" xr2:uid="{DE1357BD-E7FA-854A-BAD7-FAF24432C206}"/>
   </bookViews>
@@ -35,9 +35,58 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="13">
+  <si>
+    <t>Recursive</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>XSmallItems</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>XSmallCapacity</t>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Memoization</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="175" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45,16 +94,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -62,14 +144,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,12 +569,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F118AEB-2512-D34A-B597-F620B8AA0E81}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
+    <col min="19" max="20" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.28050000000000003</v>
+      </c>
+      <c r="D5" s="1">
+        <v>89</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.31019999999999998</v>
+      </c>
+      <c r="K5" s="1">
+        <v>89</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>1.3199000000000001</v>
+      </c>
+      <c r="R5" s="1">
+        <v>89</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>83.575500000000005</v>
+      </c>
+      <c r="D6" s="1">
+        <v>200</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="K6" s="1">
+        <v>200</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>2.0024999999999999</v>
+      </c>
+      <c r="R6" s="1">
+        <v>200</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>572.87199999999996</v>
+      </c>
+      <c r="D7" s="1">
+        <v>234</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.43840000000000001</v>
+      </c>
+      <c r="K7" s="1">
+        <v>234</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="1">
+        <v>3</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>2.3401999999999998</v>
+      </c>
+      <c r="R7" s="1">
+        <v>234</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13">
+        <v>428.15600000000001</v>
+      </c>
+      <c r="D8" s="12">
+        <v>188</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.37519999999999998</v>
+      </c>
+      <c r="K8" s="1">
+        <v>188</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="1">
+        <v>4</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>2.0145</v>
+      </c>
+      <c r="R8" s="1">
+        <v>188</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>5</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16">
+        <v>172.6566</v>
+      </c>
+      <c r="D9" s="15">
+        <v>206</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="15">
+        <v>5</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.71779999999999999</v>
+      </c>
+      <c r="K9" s="15">
+        <v>206</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="15">
+        <v>5</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>3.7122000000000002</v>
+      </c>
+      <c r="R9" s="15">
+        <v>206</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F3"/>
+    <mergeCell ref="H2:M3"/>
+    <mergeCell ref="O2:T3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added unit tests and an embeded repo
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbalkovec/Desktop/CPSC4100/FinalProject/FinalProject4100/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC416A9-FEE6-664C-87E0-8E7B172CDB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD50CD2B-8152-D447-9198-C390A1EBE9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="27700" windowHeight="17500" activeTab="1" xr2:uid="{DE1357BD-E7FA-854A-BAD7-FAF24432C206}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" activeTab="2" xr2:uid="{DE1357BD-E7FA-854A-BAD7-FAF24432C206}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual" sheetId="1" r:id="rId1"/>
     <sheet name="Raw" sheetId="2" r:id="rId2"/>
+    <sheet name="Unit Tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="60">
   <si>
     <t>Recursive</t>
   </si>
@@ -143,6 +144,81 @@
   <si>
     <t>SolutionRecursive</t>
   </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackRecursiveThreading_WithMaxCapacity_ShouldReturnMaxValue'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success </t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackMemo_WithMaxCapacity_ShouldReturnMaxValue</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackDP_WithMaxCapacity_ShouldReturnMaxValue</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackRecursive_WithMaxCapacity_ShouldReturnMaxValue</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackRecursiveThreading_WithZeroCapacity_ShouldReturnZero</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackMemo_WithZeroCapacity_ShouldReturnZero</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackDP_WithZeroCapacity_ShouldReturnZero</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackRecursive_WithEmptyItemsList_ShouldReturnZero</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackRecursive_WithZeroCapacity_ShouldReturnZero</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackRecursiveThreading_ShouldReturnCorrectValue</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackMemo_ShouldReturnCorrectValue</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackDP_ShouldReturnCorrectValue</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.KnapsackTests.KnapsackRecursive_ShouldReturnCorrectValue</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Solution_InvalidLogType_ThrowsArgumentException</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Time_InvalidLogType_ThrowsArgumentException</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Error_InvalidLogType_ThrowsArgumentException</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Info_InvalidLogType_ThrowsArgumentException</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.ClearLog_ClearsExecutionLogFile</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Solution_LogExecutionSolution_LogsSolutionMessageCorrectly</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Time_LogExecutionTime_LogsTimeMessageCorrectly'</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Error_LogOtherError_LogsErrorMessageCorrectly'</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Error_LogExecutionError_LogsErrorMessageCorrectly</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Info_LogOtherInfo_LogsInfoMessageCorrectly</t>
+  </si>
+  <si>
+    <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Info_LogExecutionInfo_LogsInfoMessageCorrectly</t>
+  </si>
 </sst>
 </file>
 
@@ -152,7 +228,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -194,8 +270,15 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,8 +363,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -825,12 +913,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1285,21 +1398,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1363,6 +1461,12 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1372,12 +1476,49 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2417,6 +2558,23 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2760,50 +2918,50 @@
   <sheetData>
     <row r="1" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:24" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="159" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="161"/>
-      <c r="K2" s="159" t="s">
+      <c r="C2" s="154" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="156"/>
+      <c r="K2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="160"/>
-      <c r="M2" s="160"/>
-      <c r="N2" s="160"/>
-      <c r="O2" s="160"/>
-      <c r="P2" s="161"/>
-      <c r="S2" s="159" t="s">
+      <c r="L2" s="155"/>
+      <c r="M2" s="155"/>
+      <c r="N2" s="155"/>
+      <c r="O2" s="155"/>
+      <c r="P2" s="156"/>
+      <c r="S2" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="160"/>
-      <c r="U2" s="160"/>
-      <c r="V2" s="160"/>
-      <c r="W2" s="160"/>
-      <c r="X2" s="161"/>
+      <c r="T2" s="155"/>
+      <c r="U2" s="155"/>
+      <c r="V2" s="155"/>
+      <c r="W2" s="155"/>
+      <c r="X2" s="156"/>
     </row>
     <row r="3" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="162"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="164"/>
-      <c r="K3" s="180"/>
-      <c r="L3" s="181"/>
-      <c r="M3" s="181"/>
-      <c r="N3" s="181"/>
-      <c r="O3" s="181"/>
-      <c r="P3" s="182"/>
-      <c r="S3" s="162"/>
-      <c r="T3" s="163"/>
-      <c r="U3" s="163"/>
-      <c r="V3" s="163"/>
-      <c r="W3" s="163"/>
-      <c r="X3" s="164"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="159"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="178"/>
+      <c r="M3" s="178"/>
+      <c r="N3" s="178"/>
+      <c r="O3" s="178"/>
+      <c r="P3" s="179"/>
+      <c r="S3" s="157"/>
+      <c r="T3" s="158"/>
+      <c r="U3" s="158"/>
+      <c r="V3" s="158"/>
+      <c r="W3" s="158"/>
+      <c r="X3" s="159"/>
     </row>
     <row r="4" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
@@ -3513,10 +3671,10 @@
     </row>
     <row r="15" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="120"/>
-      <c r="C15" s="157" t="s">
+      <c r="C15" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="158"/>
+      <c r="D15" s="176"/>
       <c r="E15" s="139">
         <f>AVERAGE(E5:E14)</f>
         <v>17.392159999999997</v>
@@ -3531,10 +3689,10 @@
         <v>71.8</v>
       </c>
       <c r="J15" s="120"/>
-      <c r="K15" s="157" t="s">
+      <c r="K15" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="158"/>
+      <c r="L15" s="176"/>
       <c r="M15" s="139">
         <f>AVERAGE(M5:M14)</f>
         <v>0.71133000000000002</v>
@@ -3549,10 +3707,10 @@
         <v>62.5</v>
       </c>
       <c r="R15" s="120"/>
-      <c r="S15" s="157" t="s">
+      <c r="S15" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="T15" s="158"/>
+      <c r="T15" s="176"/>
       <c r="U15" s="140">
         <f>AVERAGE(U5:U14)</f>
         <v>0.12404999999999999</v>
@@ -4219,10 +4377,10 @@
     </row>
     <row r="26" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="120"/>
-      <c r="C26" s="157" t="s">
+      <c r="C26" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="158"/>
+      <c r="D26" s="176"/>
       <c r="E26" s="140">
         <f>AVERAGE(E16:E25)</f>
         <v>44785.458460000002</v>
@@ -4237,10 +4395,10 @@
         <v>75.900000000000006</v>
       </c>
       <c r="J26" s="120"/>
-      <c r="K26" s="157" t="s">
+      <c r="K26" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="158"/>
+      <c r="L26" s="176"/>
       <c r="M26" s="140">
         <f>AVERAGE(M16:M25)</f>
         <v>1.0383599999999999</v>
@@ -4255,10 +4413,10 @@
         <v>76.7</v>
       </c>
       <c r="R26" s="120"/>
-      <c r="S26" s="157" t="s">
+      <c r="S26" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="158"/>
+      <c r="T26" s="176"/>
       <c r="U26" s="140">
         <f>AVERAGE(U16:U25)</f>
         <v>0.28898000000000007</v>
@@ -4925,10 +5083,10 @@
     </row>
     <row r="37" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="120"/>
-      <c r="C37" s="157" t="s">
+      <c r="C37" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="158"/>
+      <c r="D37" s="176"/>
       <c r="E37" s="140">
         <f>AVERAGE(E27:E36)</f>
         <v>-1</v>
@@ -4943,10 +5101,10 @@
         <v>62.6</v>
       </c>
       <c r="J37" s="120"/>
-      <c r="K37" s="157" t="s">
+      <c r="K37" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="L37" s="158"/>
+      <c r="L37" s="176"/>
       <c r="M37" s="140">
         <f>AVERAGE(M27:M36)</f>
         <v>2.0703299999999998</v>
@@ -4961,10 +5119,10 @@
         <v>67.2</v>
       </c>
       <c r="R37" s="120"/>
-      <c r="S37" s="157" t="s">
+      <c r="S37" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="T37" s="158"/>
+      <c r="T37" s="176"/>
       <c r="U37" s="140">
         <f>AVERAGE(U27:U36)</f>
         <v>6.5949999999999995E-2</v>
@@ -5631,10 +5789,10 @@
     </row>
     <row r="48" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="120"/>
-      <c r="C48" s="157" t="s">
+      <c r="C48" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="158"/>
+      <c r="D48" s="176"/>
       <c r="E48" s="140">
         <f>AVERAGE(E38:E47)</f>
         <v>-1</v>
@@ -5649,10 +5807,10 @@
         <v>74.400000000000006</v>
       </c>
       <c r="J48" s="120"/>
-      <c r="K48" s="157" t="s">
+      <c r="K48" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="158"/>
+      <c r="L48" s="176"/>
       <c r="M48" s="140">
         <f>AVERAGE(M38:M47)</f>
         <v>3.8687499999999999</v>
@@ -5667,10 +5825,10 @@
         <v>69.900000000000006</v>
       </c>
       <c r="R48" s="120"/>
-      <c r="S48" s="157" t="s">
+      <c r="S48" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="T48" s="158"/>
+      <c r="T48" s="176"/>
       <c r="U48" s="140">
         <f>AVERAGE(U38:U47)</f>
         <v>0.19390999999999997</v>
@@ -6336,10 +6494,10 @@
       </c>
     </row>
     <row r="59" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="157" t="s">
+      <c r="C59" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="158"/>
+      <c r="D59" s="176"/>
       <c r="E59" s="140">
         <f>AVERAGE(E49:E58)</f>
         <v>-1</v>
@@ -6353,10 +6511,10 @@
         <f>AVERAGE(H49:H58)</f>
         <v>66.2</v>
       </c>
-      <c r="K59" s="157" t="s">
+      <c r="K59" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="L59" s="158"/>
+      <c r="L59" s="176"/>
       <c r="M59" s="140">
         <f>AVERAGE(M49:M58)</f>
         <v>10.25055</v>
@@ -6370,10 +6528,10 @@
         <f>AVERAGE(P49:P58)</f>
         <v>62.5</v>
       </c>
-      <c r="S59" s="157" t="s">
+      <c r="S59" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="T59" s="158"/>
+      <c r="T59" s="176"/>
       <c r="U59" s="140">
         <f>AVERAGE(U49:U58)</f>
         <v>0.25315000000000004</v>
@@ -6390,37 +6548,37 @@
     </row>
     <row r="61" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C62" s="165" t="s">
+      <c r="C62" s="160" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="166"/>
-      <c r="E62" s="166"/>
-      <c r="F62" s="167"/>
+      <c r="D62" s="161"/>
+      <c r="E62" s="161"/>
+      <c r="F62" s="162"/>
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="C63" s="168"/>
-      <c r="D63" s="169"/>
-      <c r="E63" s="169"/>
-      <c r="F63" s="170"/>
+      <c r="C63" s="163"/>
+      <c r="D63" s="164"/>
+      <c r="E63" s="164"/>
+      <c r="F63" s="165"/>
     </row>
     <row r="64" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="171"/>
-      <c r="D64" s="172"/>
-      <c r="E64" s="172"/>
-      <c r="F64" s="173"/>
+      <c r="C64" s="166"/>
+      <c r="D64" s="167"/>
+      <c r="E64" s="167"/>
+      <c r="F64" s="168"/>
     </row>
     <row r="65" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="3:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="174" t="s">
+      <c r="C66" s="169" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="175"/>
-      <c r="E66" s="176"/>
+      <c r="D66" s="170"/>
+      <c r="E66" s="171"/>
     </row>
     <row r="67" spans="3:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="177"/>
-      <c r="D67" s="178"/>
-      <c r="E67" s="179"/>
+      <c r="C67" s="172"/>
+      <c r="D67" s="173"/>
+      <c r="E67" s="174"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C68" s="81" t="s">
@@ -6480,15 +6638,22 @@
     </row>
     <row r="74" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="154" t="s">
+      <c r="C75" s="180" t="s">
         <v>22</v>
       </c>
-      <c r="D75" s="155"/>
-      <c r="E75" s="155"/>
-      <c r="F75" s="156"/>
+      <c r="D75" s="181"/>
+      <c r="E75" s="181"/>
+      <c r="F75" s="182"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="S59:T59"/>
     <mergeCell ref="S2:X3"/>
     <mergeCell ref="C2:H3"/>
     <mergeCell ref="C62:F64"/>
@@ -6503,13 +6668,6 @@
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="K48:L48"/>
     <mergeCell ref="K2:P3"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="S59:T59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6520,7 +6678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4168ABF-7E0F-0044-AD3D-7783777C6A22}">
   <dimension ref="A2:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -6599,7 +6757,7 @@
       <c r="H3" s="149">
         <v>11.975199999999999</v>
       </c>
-      <c r="I3" s="183">
+      <c r="I3" s="152">
         <v>65</v>
       </c>
       <c r="J3" s="147">
@@ -6634,7 +6792,7 @@
       <c r="H4" s="149">
         <v>8.2377000000000002</v>
       </c>
-      <c r="I4" s="183">
+      <c r="I4" s="152">
         <v>74</v>
       </c>
       <c r="J4" s="147">
@@ -6669,7 +6827,7 @@
       <c r="H5" s="149">
         <v>0.20069999999999999</v>
       </c>
-      <c r="I5" s="183">
+      <c r="I5" s="152">
         <v>44</v>
       </c>
       <c r="J5" s="147">
@@ -6704,7 +6862,7 @@
       <c r="H6" s="149">
         <v>8.2539999999999996</v>
       </c>
-      <c r="I6" s="183">
+      <c r="I6" s="152">
         <v>74</v>
       </c>
       <c r="J6" s="147">
@@ -6739,7 +6897,7 @@
       <c r="H7" s="149">
         <v>0.30759999999999998</v>
       </c>
-      <c r="I7" s="183">
+      <c r="I7" s="152">
         <v>47</v>
       </c>
       <c r="J7" s="147">
@@ -6774,7 +6932,7 @@
       <c r="H8" s="149">
         <v>22.0045</v>
       </c>
-      <c r="I8" s="183">
+      <c r="I8" s="152">
         <v>89</v>
       </c>
       <c r="J8" s="147">
@@ -6809,7 +6967,7 @@
       <c r="H9" s="149">
         <v>0.46260000000000001</v>
       </c>
-      <c r="I9" s="183">
+      <c r="I9" s="152">
         <v>64</v>
       </c>
       <c r="J9" s="147">
@@ -6844,7 +7002,7 @@
       <c r="H10" s="150">
         <v>106.7842</v>
       </c>
-      <c r="I10" s="183">
+      <c r="I10" s="152">
         <v>119</v>
       </c>
       <c r="J10" s="147">
@@ -6879,7 +7037,7 @@
       <c r="H11" s="150">
         <v>15.649100000000001</v>
       </c>
-      <c r="I11" s="183">
+      <c r="I11" s="152">
         <v>98</v>
       </c>
       <c r="J11" s="147">
@@ -6914,7 +7072,7 @@
       <c r="H12" s="150">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="I12" s="183">
+      <c r="I12" s="152">
         <v>44</v>
       </c>
       <c r="J12" s="147">
@@ -6949,7 +7107,7 @@
       <c r="H13" s="149">
         <v>6679.2203</v>
       </c>
-      <c r="I13" s="183">
+      <c r="I13" s="152">
         <v>84</v>
       </c>
       <c r="J13" s="147">
@@ -6984,7 +7142,7 @@
       <c r="H14" s="149">
         <v>276.4384</v>
       </c>
-      <c r="I14" s="183">
+      <c r="I14" s="152">
         <v>65</v>
       </c>
       <c r="J14" s="147">
@@ -7019,7 +7177,7 @@
       <c r="H15" s="149">
         <v>22679.67</v>
       </c>
-      <c r="I15" s="183">
+      <c r="I15" s="152">
         <v>92</v>
       </c>
       <c r="J15" s="147">
@@ -7054,7 +7212,7 @@
       <c r="H16" s="149">
         <v>6668.933</v>
       </c>
-      <c r="I16" s="183">
+      <c r="I16" s="152">
         <v>84</v>
       </c>
       <c r="J16" s="147">
@@ -7089,7 +7247,7 @@
       <c r="H17" s="149">
         <v>310926.12319999997</v>
       </c>
-      <c r="I17" s="183">
+      <c r="I17" s="152">
         <v>110</v>
       </c>
       <c r="J17" s="147">
@@ -7124,7 +7282,7 @@
       <c r="H18" s="150">
         <v>85928.341400000005</v>
       </c>
-      <c r="I18" s="183">
+      <c r="I18" s="152">
         <v>113</v>
       </c>
       <c r="J18" s="147">
@@ -7159,7 +7317,7 @@
       <c r="H19" s="150">
         <v>5.9802</v>
       </c>
-      <c r="I19" s="183">
+      <c r="I19" s="152">
         <v>51</v>
       </c>
       <c r="J19" s="147">
@@ -7194,7 +7352,7 @@
       <c r="H20" s="150">
         <v>0.19370000000000001</v>
       </c>
-      <c r="I20" s="183">
+      <c r="I20" s="152">
         <v>33</v>
       </c>
       <c r="J20" s="147">
@@ -7229,7 +7387,7 @@
       <c r="H21" s="150">
         <v>6.0100000000000001E-2</v>
       </c>
-      <c r="I21" s="183">
+      <c r="I21" s="152">
         <v>27</v>
       </c>
       <c r="J21" s="147">
@@ -7264,7 +7422,7 @@
       <c r="H22" s="150">
         <v>14689.624299999999</v>
       </c>
-      <c r="I22" s="183">
+      <c r="I22" s="152">
         <v>100</v>
       </c>
       <c r="J22" s="147">
@@ -8336,4 +8494,1399 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074BBD8A-C58A-6D43-AB50-6FAB8ACE68BE}">
+  <dimension ref="C1:M78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="192"/>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C3" s="187"/>
+      <c r="D3" s="188" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="151"/>
+      <c r="M3" s="184"/>
+    </row>
+    <row r="4" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="187"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
+      <c r="I4" s="151"/>
+      <c r="J4" s="151"/>
+      <c r="K4" s="151"/>
+      <c r="L4" s="151"/>
+      <c r="M4" s="184"/>
+    </row>
+    <row r="5" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="151"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
+      <c r="H5" s="151"/>
+      <c r="I5" s="151"/>
+      <c r="J5" s="151"/>
+      <c r="K5" s="151"/>
+      <c r="L5" s="151"/>
+      <c r="M5" s="184"/>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C6" s="187"/>
+      <c r="D6" s="188" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="188"/>
+      <c r="F6" s="188"/>
+      <c r="G6" s="188"/>
+      <c r="H6" s="188"/>
+      <c r="I6" s="188"/>
+      <c r="J6" s="188"/>
+      <c r="K6" s="188"/>
+      <c r="L6" s="151"/>
+      <c r="M6" s="184"/>
+    </row>
+    <row r="7" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="187"/>
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="151"/>
+      <c r="L7" s="151"/>
+      <c r="M7" s="184"/>
+    </row>
+    <row r="8" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="151"/>
+      <c r="F8" s="151"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="151"/>
+      <c r="I8" s="151"/>
+      <c r="J8" s="151"/>
+      <c r="K8" s="151"/>
+      <c r="L8" s="151"/>
+      <c r="M8" s="184"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C9" s="187"/>
+      <c r="D9" s="188" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="188"/>
+      <c r="F9" s="188"/>
+      <c r="G9" s="188"/>
+      <c r="H9" s="188"/>
+      <c r="I9" s="188"/>
+      <c r="J9" s="188"/>
+      <c r="K9" s="188"/>
+      <c r="L9" s="151"/>
+      <c r="M9" s="184"/>
+    </row>
+    <row r="10" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="187"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="151"/>
+      <c r="G10" s="151"/>
+      <c r="H10" s="151"/>
+      <c r="I10" s="151"/>
+      <c r="J10" s="151"/>
+      <c r="K10" s="151"/>
+      <c r="L10" s="151"/>
+      <c r="M10" s="184"/>
+    </row>
+    <row r="11" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
+      <c r="G11" s="151"/>
+      <c r="H11" s="151"/>
+      <c r="I11" s="151"/>
+      <c r="J11" s="151"/>
+      <c r="K11" s="151"/>
+      <c r="L11" s="151"/>
+      <c r="M11" s="184"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C12" s="187"/>
+      <c r="D12" s="188" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="151"/>
+      <c r="K12" s="151"/>
+      <c r="L12" s="151"/>
+      <c r="M12" s="184"/>
+    </row>
+    <row r="13" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="187"/>
+      <c r="D13" s="151"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="151"/>
+      <c r="G13" s="151"/>
+      <c r="H13" s="151"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="151"/>
+      <c r="K13" s="151"/>
+      <c r="L13" s="151"/>
+      <c r="M13" s="184"/>
+    </row>
+    <row r="14" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
+      <c r="G14" s="151"/>
+      <c r="H14" s="151"/>
+      <c r="I14" s="151"/>
+      <c r="J14" s="151"/>
+      <c r="K14" s="151"/>
+      <c r="L14" s="151"/>
+      <c r="M14" s="184"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C15" s="187"/>
+      <c r="D15" s="151" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="184"/>
+    </row>
+    <row r="16" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="187"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
+      <c r="M16" s="184"/>
+    </row>
+    <row r="17" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
+      <c r="G17" s="151"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="151"/>
+      <c r="L17" s="151"/>
+      <c r="M17" s="184"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C18" s="187"/>
+      <c r="D18" s="151" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="151"/>
+      <c r="J18" s="151"/>
+      <c r="K18" s="151"/>
+      <c r="L18" s="151"/>
+      <c r="M18" s="184"/>
+    </row>
+    <row r="19" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="187"/>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="151"/>
+      <c r="K19" s="151"/>
+      <c r="L19" s="151"/>
+      <c r="M19" s="184"/>
+    </row>
+    <row r="20" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="151"/>
+      <c r="K20" s="151"/>
+      <c r="L20" s="151"/>
+      <c r="M20" s="184"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C21" s="187"/>
+      <c r="D21" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="151"/>
+      <c r="F21" s="151"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="151"/>
+      <c r="J21" s="151"/>
+      <c r="K21" s="151"/>
+      <c r="L21" s="151"/>
+      <c r="M21" s="184"/>
+    </row>
+    <row r="22" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="187"/>
+      <c r="D22" s="151"/>
+      <c r="E22" s="151"/>
+      <c r="F22" s="151"/>
+      <c r="G22" s="151"/>
+      <c r="H22" s="151"/>
+      <c r="I22" s="151"/>
+      <c r="J22" s="151"/>
+      <c r="K22" s="151"/>
+      <c r="L22" s="151"/>
+      <c r="M22" s="184"/>
+    </row>
+    <row r="23" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="151"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
+      <c r="J23" s="151"/>
+      <c r="K23" s="151"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="184"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C24" s="187"/>
+      <c r="D24" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="151"/>
+      <c r="F24" s="151"/>
+      <c r="G24" s="151"/>
+      <c r="H24" s="151"/>
+      <c r="I24" s="151"/>
+      <c r="J24" s="151"/>
+      <c r="K24" s="151"/>
+      <c r="L24" s="151"/>
+      <c r="M24" s="184"/>
+    </row>
+    <row r="25" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="187"/>
+      <c r="D25" s="151"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="151"/>
+      <c r="G25" s="151"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
+      <c r="J25" s="151"/>
+      <c r="K25" s="151"/>
+      <c r="L25" s="151"/>
+      <c r="M25" s="184"/>
+    </row>
+    <row r="26" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="151"/>
+      <c r="F26" s="151"/>
+      <c r="G26" s="151"/>
+      <c r="H26" s="151"/>
+      <c r="I26" s="151"/>
+      <c r="J26" s="151"/>
+      <c r="K26" s="151"/>
+      <c r="L26" s="151"/>
+      <c r="M26" s="184"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C27" s="187"/>
+      <c r="D27" s="151" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="151"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="151"/>
+      <c r="K27" s="151"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="184"/>
+    </row>
+    <row r="28" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="187"/>
+      <c r="D28" s="151"/>
+      <c r="E28" s="151"/>
+      <c r="F28" s="151"/>
+      <c r="G28" s="151"/>
+      <c r="H28" s="151"/>
+      <c r="I28" s="151"/>
+      <c r="J28" s="151"/>
+      <c r="K28" s="151"/>
+      <c r="L28" s="151"/>
+      <c r="M28" s="184"/>
+    </row>
+    <row r="29" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="151"/>
+      <c r="F29" s="151"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="151"/>
+      <c r="K29" s="151"/>
+      <c r="L29" s="151"/>
+      <c r="M29" s="184"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C30" s="187"/>
+      <c r="D30" s="151" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="151"/>
+      <c r="F30" s="151"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="151"/>
+      <c r="K30" s="151"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="184"/>
+    </row>
+    <row r="31" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="187"/>
+      <c r="D31" s="151"/>
+      <c r="E31" s="151"/>
+      <c r="F31" s="151"/>
+      <c r="G31" s="151"/>
+      <c r="H31" s="151"/>
+      <c r="I31" s="151"/>
+      <c r="J31" s="151"/>
+      <c r="K31" s="151"/>
+      <c r="L31" s="151"/>
+      <c r="M31" s="184"/>
+    </row>
+    <row r="32" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
+      <c r="G32" s="151"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="151"/>
+      <c r="K32" s="151"/>
+      <c r="L32" s="151"/>
+      <c r="M32" s="184"/>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C33" s="187"/>
+      <c r="D33" s="151" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="151"/>
+      <c r="F33" s="151"/>
+      <c r="G33" s="151"/>
+      <c r="H33" s="151"/>
+      <c r="I33" s="151"/>
+      <c r="J33" s="151"/>
+      <c r="K33" s="151"/>
+      <c r="L33" s="151"/>
+      <c r="M33" s="184"/>
+    </row>
+    <row r="34" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="187"/>
+      <c r="D34" s="151"/>
+      <c r="E34" s="151"/>
+      <c r="F34" s="151"/>
+      <c r="G34" s="151"/>
+      <c r="H34" s="151"/>
+      <c r="I34" s="151"/>
+      <c r="J34" s="151"/>
+      <c r="K34" s="151"/>
+      <c r="L34" s="151"/>
+      <c r="M34" s="184"/>
+    </row>
+    <row r="35" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="151"/>
+      <c r="F35" s="151"/>
+      <c r="G35" s="151"/>
+      <c r="H35" s="151"/>
+      <c r="I35" s="151"/>
+      <c r="J35" s="151"/>
+      <c r="K35" s="151"/>
+      <c r="L35" s="151"/>
+      <c r="M35" s="184"/>
+    </row>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C36" s="187"/>
+      <c r="D36" s="151" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="151"/>
+      <c r="F36" s="151"/>
+      <c r="G36" s="151"/>
+      <c r="H36" s="151"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="151"/>
+      <c r="K36" s="151"/>
+      <c r="L36" s="151"/>
+      <c r="M36" s="184"/>
+    </row>
+    <row r="37" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="187"/>
+      <c r="D37" s="151"/>
+      <c r="E37" s="151"/>
+      <c r="F37" s="151"/>
+      <c r="G37" s="151"/>
+      <c r="H37" s="151"/>
+      <c r="I37" s="151"/>
+      <c r="J37" s="151"/>
+      <c r="K37" s="151"/>
+      <c r="L37" s="151"/>
+      <c r="M37" s="184"/>
+    </row>
+    <row r="38" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="151"/>
+      <c r="F38" s="151"/>
+      <c r="G38" s="151"/>
+      <c r="H38" s="151"/>
+      <c r="I38" s="151"/>
+      <c r="J38" s="151"/>
+      <c r="K38" s="151"/>
+      <c r="L38" s="151"/>
+      <c r="M38" s="184"/>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C39" s="187"/>
+      <c r="D39" s="151" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="151"/>
+      <c r="F39" s="151"/>
+      <c r="G39" s="151"/>
+      <c r="H39" s="151"/>
+      <c r="I39" s="151"/>
+      <c r="J39" s="151"/>
+      <c r="K39" s="151"/>
+      <c r="L39" s="151"/>
+      <c r="M39" s="184"/>
+    </row>
+    <row r="40" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="187"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="151"/>
+      <c r="F40" s="151"/>
+      <c r="G40" s="151"/>
+      <c r="H40" s="151"/>
+      <c r="I40" s="151"/>
+      <c r="J40" s="151"/>
+      <c r="K40" s="151"/>
+      <c r="L40" s="151"/>
+      <c r="M40" s="184"/>
+    </row>
+    <row r="41" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="151"/>
+      <c r="F41" s="151"/>
+      <c r="G41" s="151"/>
+      <c r="H41" s="151"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="151"/>
+      <c r="K41" s="151"/>
+      <c r="L41" s="151"/>
+      <c r="M41" s="184"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C42" s="187"/>
+      <c r="D42" s="151" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="151"/>
+      <c r="F42" s="151"/>
+      <c r="G42" s="151"/>
+      <c r="H42" s="151"/>
+      <c r="I42" s="151"/>
+      <c r="J42" s="151"/>
+      <c r="K42" s="151"/>
+      <c r="L42" s="151"/>
+      <c r="M42" s="184"/>
+    </row>
+    <row r="43" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="187"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="151"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="151"/>
+      <c r="J43" s="151"/>
+      <c r="K43" s="151"/>
+      <c r="L43" s="151"/>
+      <c r="M43" s="184"/>
+    </row>
+    <row r="44" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="151"/>
+      <c r="F44" s="151"/>
+      <c r="G44" s="151"/>
+      <c r="H44" s="151"/>
+      <c r="I44" s="151"/>
+      <c r="J44" s="151"/>
+      <c r="K44" s="151"/>
+      <c r="L44" s="151"/>
+      <c r="M44" s="184"/>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C45" s="187"/>
+      <c r="D45" s="151" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" s="151"/>
+      <c r="F45" s="151"/>
+      <c r="G45" s="151"/>
+      <c r="H45" s="151"/>
+      <c r="I45" s="151"/>
+      <c r="J45" s="151"/>
+      <c r="K45" s="151"/>
+      <c r="L45" s="151"/>
+      <c r="M45" s="184"/>
+    </row>
+    <row r="46" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="187"/>
+      <c r="D46" s="151"/>
+      <c r="E46" s="151"/>
+      <c r="F46" s="151"/>
+      <c r="G46" s="151"/>
+      <c r="H46" s="151"/>
+      <c r="I46" s="151"/>
+      <c r="J46" s="151"/>
+      <c r="K46" s="151"/>
+      <c r="L46" s="151"/>
+      <c r="M46" s="184"/>
+    </row>
+    <row r="47" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="151"/>
+      <c r="F47" s="151"/>
+      <c r="G47" s="151"/>
+      <c r="H47" s="151"/>
+      <c r="I47" s="151"/>
+      <c r="J47" s="151"/>
+      <c r="K47" s="151"/>
+      <c r="L47" s="151"/>
+      <c r="M47" s="184"/>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C48" s="187"/>
+      <c r="D48" s="151" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="151"/>
+      <c r="F48" s="151"/>
+      <c r="G48" s="151"/>
+      <c r="H48" s="151"/>
+      <c r="I48" s="151"/>
+      <c r="J48" s="151"/>
+      <c r="K48" s="151"/>
+      <c r="L48" s="151"/>
+      <c r="M48" s="184"/>
+    </row>
+    <row r="49" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="187"/>
+      <c r="D49" s="151"/>
+      <c r="E49" s="151"/>
+      <c r="F49" s="151"/>
+      <c r="G49" s="151"/>
+      <c r="H49" s="151"/>
+      <c r="I49" s="151"/>
+      <c r="J49" s="151"/>
+      <c r="K49" s="151"/>
+      <c r="L49" s="151"/>
+      <c r="M49" s="184"/>
+    </row>
+    <row r="50" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="151"/>
+      <c r="F50" s="151"/>
+      <c r="G50" s="151"/>
+      <c r="H50" s="151"/>
+      <c r="I50" s="151"/>
+      <c r="J50" s="151"/>
+      <c r="K50" s="151"/>
+      <c r="L50" s="151"/>
+      <c r="M50" s="184"/>
+    </row>
+    <row r="51" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C51" s="187"/>
+      <c r="D51" s="151" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="151"/>
+      <c r="F51" s="151"/>
+      <c r="G51" s="151"/>
+      <c r="H51" s="151"/>
+      <c r="I51" s="151"/>
+      <c r="J51" s="151"/>
+      <c r="K51" s="151"/>
+      <c r="L51" s="151"/>
+      <c r="M51" s="184"/>
+    </row>
+    <row r="52" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="187"/>
+      <c r="D52" s="151"/>
+      <c r="E52" s="151"/>
+      <c r="F52" s="151"/>
+      <c r="G52" s="151"/>
+      <c r="H52" s="151"/>
+      <c r="I52" s="151"/>
+      <c r="J52" s="151"/>
+      <c r="K52" s="151"/>
+      <c r="L52" s="151"/>
+      <c r="M52" s="184"/>
+    </row>
+    <row r="53" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="151"/>
+      <c r="F53" s="151"/>
+      <c r="G53" s="151"/>
+      <c r="H53" s="151"/>
+      <c r="I53" s="151"/>
+      <c r="J53" s="151"/>
+      <c r="K53" s="151"/>
+      <c r="L53" s="151"/>
+      <c r="M53" s="184"/>
+    </row>
+    <row r="54" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C54" s="187"/>
+      <c r="D54" s="151" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="151"/>
+      <c r="F54" s="151"/>
+      <c r="G54" s="151"/>
+      <c r="H54" s="151"/>
+      <c r="I54" s="151"/>
+      <c r="J54" s="151"/>
+      <c r="K54" s="151"/>
+      <c r="L54" s="151"/>
+      <c r="M54" s="184"/>
+    </row>
+    <row r="55" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="187"/>
+      <c r="D55" s="151"/>
+      <c r="E55" s="151"/>
+      <c r="F55" s="151"/>
+      <c r="G55" s="151"/>
+      <c r="H55" s="151"/>
+      <c r="I55" s="151"/>
+      <c r="J55" s="151"/>
+      <c r="K55" s="151"/>
+      <c r="L55" s="151"/>
+      <c r="M55" s="184"/>
+    </row>
+    <row r="56" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="151"/>
+      <c r="F56" s="151"/>
+      <c r="G56" s="151"/>
+      <c r="H56" s="151"/>
+      <c r="I56" s="151"/>
+      <c r="J56" s="151"/>
+      <c r="K56" s="151"/>
+      <c r="L56" s="151"/>
+      <c r="M56" s="184"/>
+    </row>
+    <row r="57" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C57" s="187"/>
+      <c r="D57" s="151" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" s="151"/>
+      <c r="F57" s="151"/>
+      <c r="G57" s="151"/>
+      <c r="H57" s="151"/>
+      <c r="I57" s="151"/>
+      <c r="J57" s="151"/>
+      <c r="K57" s="151"/>
+      <c r="L57" s="151"/>
+      <c r="M57" s="184"/>
+    </row>
+    <row r="58" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="187"/>
+      <c r="D58" s="151"/>
+      <c r="E58" s="151"/>
+      <c r="F58" s="151"/>
+      <c r="G58" s="151"/>
+      <c r="H58" s="151"/>
+      <c r="I58" s="151"/>
+      <c r="J58" s="151"/>
+      <c r="K58" s="151"/>
+      <c r="L58" s="151"/>
+      <c r="M58" s="184"/>
+    </row>
+    <row r="59" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="151"/>
+      <c r="F59" s="151"/>
+      <c r="G59" s="151"/>
+      <c r="H59" s="151"/>
+      <c r="I59" s="151"/>
+      <c r="J59" s="151"/>
+      <c r="K59" s="151"/>
+      <c r="L59" s="151"/>
+      <c r="M59" s="184"/>
+    </row>
+    <row r="60" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C60" s="187"/>
+      <c r="D60" s="151" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="151"/>
+      <c r="F60" s="151"/>
+      <c r="G60" s="151"/>
+      <c r="H60" s="151"/>
+      <c r="I60" s="151"/>
+      <c r="J60" s="151"/>
+      <c r="K60" s="151"/>
+      <c r="L60" s="151"/>
+      <c r="M60" s="184"/>
+    </row>
+    <row r="61" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="187"/>
+      <c r="D61" s="151"/>
+      <c r="E61" s="151"/>
+      <c r="F61" s="151"/>
+      <c r="G61" s="151"/>
+      <c r="H61" s="151"/>
+      <c r="I61" s="151"/>
+      <c r="J61" s="151"/>
+      <c r="K61" s="151"/>
+      <c r="L61" s="151"/>
+      <c r="M61" s="184"/>
+    </row>
+    <row r="62" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="151"/>
+      <c r="F62" s="151"/>
+      <c r="G62" s="151"/>
+      <c r="H62" s="151"/>
+      <c r="I62" s="151"/>
+      <c r="J62" s="151"/>
+      <c r="K62" s="151"/>
+      <c r="L62" s="151"/>
+      <c r="M62" s="184"/>
+    </row>
+    <row r="63" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C63" s="187"/>
+      <c r="D63" s="151" t="s">
+        <v>39</v>
+      </c>
+      <c r="E63" s="151"/>
+      <c r="F63" s="151"/>
+      <c r="G63" s="151"/>
+      <c r="H63" s="151"/>
+      <c r="I63" s="151"/>
+      <c r="J63" s="151"/>
+      <c r="K63" s="151"/>
+      <c r="L63" s="151"/>
+      <c r="M63" s="184"/>
+    </row>
+    <row r="64" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="187"/>
+      <c r="D64" s="151"/>
+      <c r="E64" s="151"/>
+      <c r="F64" s="151"/>
+      <c r="G64" s="151"/>
+      <c r="H64" s="151"/>
+      <c r="I64" s="151"/>
+      <c r="J64" s="151"/>
+      <c r="K64" s="151"/>
+      <c r="L64" s="151"/>
+      <c r="M64" s="184"/>
+    </row>
+    <row r="65" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="151"/>
+      <c r="F65" s="151"/>
+      <c r="G65" s="151"/>
+      <c r="H65" s="151"/>
+      <c r="I65" s="151"/>
+      <c r="J65" s="151"/>
+      <c r="K65" s="151"/>
+      <c r="L65" s="151"/>
+      <c r="M65" s="184"/>
+    </row>
+    <row r="66" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C66" s="187"/>
+      <c r="D66" s="151" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="151"/>
+      <c r="F66" s="151"/>
+      <c r="G66" s="151"/>
+      <c r="H66" s="151"/>
+      <c r="I66" s="151"/>
+      <c r="J66" s="151"/>
+      <c r="K66" s="151"/>
+      <c r="L66" s="151"/>
+      <c r="M66" s="184"/>
+    </row>
+    <row r="67" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="187"/>
+      <c r="D67" s="151"/>
+      <c r="E67" s="151"/>
+      <c r="F67" s="151"/>
+      <c r="G67" s="151"/>
+      <c r="H67" s="151"/>
+      <c r="I67" s="151"/>
+      <c r="J67" s="151"/>
+      <c r="K67" s="151"/>
+      <c r="L67" s="151"/>
+      <c r="M67" s="184"/>
+    </row>
+    <row r="68" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" s="151"/>
+      <c r="F68" s="151"/>
+      <c r="G68" s="151"/>
+      <c r="H68" s="151"/>
+      <c r="I68" s="151"/>
+      <c r="J68" s="151"/>
+      <c r="K68" s="151"/>
+      <c r="L68" s="151"/>
+      <c r="M68" s="184"/>
+    </row>
+    <row r="69" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C69" s="187"/>
+      <c r="D69" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="E69" s="151"/>
+      <c r="F69" s="151"/>
+      <c r="G69" s="151"/>
+      <c r="H69" s="151"/>
+      <c r="I69" s="151"/>
+      <c r="J69" s="151"/>
+      <c r="K69" s="151"/>
+      <c r="L69" s="151"/>
+      <c r="M69" s="184"/>
+    </row>
+    <row r="70" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="187"/>
+      <c r="D70" s="151"/>
+      <c r="E70" s="151"/>
+      <c r="F70" s="151"/>
+      <c r="G70" s="151"/>
+      <c r="H70" s="151"/>
+      <c r="I70" s="151"/>
+      <c r="J70" s="151"/>
+      <c r="K70" s="151"/>
+      <c r="L70" s="151"/>
+      <c r="M70" s="184"/>
+    </row>
+    <row r="71" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" s="151"/>
+      <c r="F71" s="151"/>
+      <c r="G71" s="151"/>
+      <c r="H71" s="151"/>
+      <c r="I71" s="151"/>
+      <c r="J71" s="151"/>
+      <c r="K71" s="151"/>
+      <c r="L71" s="151"/>
+      <c r="M71" s="184"/>
+    </row>
+    <row r="72" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="183"/>
+      <c r="D72" s="189" t="s">
+        <v>35</v>
+      </c>
+      <c r="E72" s="189"/>
+      <c r="F72" s="189"/>
+      <c r="G72" s="189"/>
+      <c r="H72" s="189"/>
+      <c r="I72" s="189"/>
+      <c r="J72" s="189"/>
+      <c r="K72" s="189"/>
+      <c r="L72" s="189"/>
+      <c r="M72" s="190"/>
+    </row>
+    <row r="73" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C73" s="151"/>
+      <c r="D73" s="151"/>
+      <c r="E73" s="151"/>
+      <c r="F73" s="151"/>
+      <c r="G73" s="151"/>
+      <c r="H73" s="151"/>
+      <c r="I73" s="151"/>
+      <c r="J73" s="151"/>
+      <c r="K73" s="151"/>
+      <c r="L73" s="151"/>
+    </row>
+    <row r="74" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C74" s="151"/>
+      <c r="D74" s="151"/>
+      <c r="E74" s="151"/>
+      <c r="F74" s="151"/>
+      <c r="G74" s="151"/>
+      <c r="H74" s="151"/>
+      <c r="I74" s="151"/>
+      <c r="J74" s="151"/>
+      <c r="K74" s="151"/>
+      <c r="L74" s="151"/>
+    </row>
+    <row r="75" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C75" s="151"/>
+      <c r="D75" s="151"/>
+      <c r="E75" s="151"/>
+      <c r="F75" s="151"/>
+      <c r="G75" s="151"/>
+      <c r="H75" s="151"/>
+      <c r="I75" s="151"/>
+      <c r="J75" s="151"/>
+      <c r="K75" s="151"/>
+      <c r="L75" s="151"/>
+    </row>
+    <row r="76" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C76" s="151"/>
+      <c r="D76" s="151"/>
+      <c r="E76" s="151"/>
+      <c r="F76" s="151"/>
+      <c r="G76" s="151"/>
+      <c r="H76" s="151"/>
+      <c r="I76" s="151"/>
+      <c r="J76" s="151"/>
+      <c r="K76" s="151"/>
+      <c r="L76" s="151"/>
+    </row>
+    <row r="77" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C77" s="151"/>
+      <c r="D77" s="151"/>
+      <c r="E77" s="151"/>
+      <c r="F77" s="151"/>
+      <c r="G77" s="151"/>
+      <c r="H77" s="151"/>
+      <c r="I77" s="151"/>
+      <c r="J77" s="151"/>
+      <c r="K77" s="151"/>
+      <c r="L77" s="151"/>
+    </row>
+    <row r="78" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C78" s="151"/>
+      <c r="D78" s="151"/>
+      <c r="E78" s="151"/>
+      <c r="F78" s="151"/>
+      <c r="G78" s="151"/>
+      <c r="H78" s="151"/>
+      <c r="I78" s="151"/>
+      <c r="J78" s="151"/>
+      <c r="K78" s="151"/>
+      <c r="L78" s="151"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes, added estimates
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbalkovec/Desktop/CPSC4100/FinalProject/FinalProject4100/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD50CD2B-8152-D447-9198-C390A1EBE9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D264B9-CF44-5944-8222-BAC57DAA3E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" activeTab="2" xr2:uid="{DE1357BD-E7FA-854A-BAD7-FAF24432C206}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" activeTab="3" xr2:uid="{DE1357BD-E7FA-854A-BAD7-FAF24432C206}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual" sheetId="1" r:id="rId1"/>
     <sheet name="Raw" sheetId="2" r:id="rId2"/>
     <sheet name="Unit Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="63">
   <si>
     <t>Recursive</t>
   </si>
@@ -219,6 +220,15 @@
   <si>
     <t>FPUnitTests.FPUnitTests.FPUnitTests.LoggerTests.Info_LogExecutionInfo_LogsInfoMessageCorrectly</t>
   </si>
+  <si>
+    <t>Median Rec</t>
+  </si>
+  <si>
+    <t>Median DP</t>
+  </si>
+  <si>
+    <t>Median Memo</t>
+  </si>
 </sst>
 </file>
 
@@ -943,7 +953,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1398,93 +1408,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1515,6 +1438,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2918,50 +2929,50 @@
   <sheetData>
     <row r="1" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:24" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="154" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="156"/>
-      <c r="K2" s="154" t="s">
+      <c r="C2" s="169" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="171"/>
+      <c r="K2" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="155"/>
-      <c r="O2" s="155"/>
-      <c r="P2" s="156"/>
-      <c r="S2" s="154" t="s">
+      <c r="L2" s="170"/>
+      <c r="M2" s="170"/>
+      <c r="N2" s="170"/>
+      <c r="O2" s="170"/>
+      <c r="P2" s="171"/>
+      <c r="S2" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="155"/>
-      <c r="U2" s="155"/>
-      <c r="V2" s="155"/>
-      <c r="W2" s="155"/>
-      <c r="X2" s="156"/>
+      <c r="T2" s="170"/>
+      <c r="U2" s="170"/>
+      <c r="V2" s="170"/>
+      <c r="W2" s="170"/>
+      <c r="X2" s="171"/>
     </row>
     <row r="3" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="157"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="159"/>
-      <c r="K3" s="177"/>
-      <c r="L3" s="178"/>
-      <c r="M3" s="178"/>
-      <c r="N3" s="178"/>
-      <c r="O3" s="178"/>
-      <c r="P3" s="179"/>
-      <c r="S3" s="157"/>
-      <c r="T3" s="158"/>
-      <c r="U3" s="158"/>
-      <c r="V3" s="158"/>
-      <c r="W3" s="158"/>
-      <c r="X3" s="159"/>
+      <c r="C3" s="172"/>
+      <c r="D3" s="173"/>
+      <c r="E3" s="173"/>
+      <c r="F3" s="173"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="174"/>
+      <c r="K3" s="190"/>
+      <c r="L3" s="191"/>
+      <c r="M3" s="191"/>
+      <c r="N3" s="191"/>
+      <c r="O3" s="191"/>
+      <c r="P3" s="192"/>
+      <c r="S3" s="172"/>
+      <c r="T3" s="173"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="173"/>
+      <c r="W3" s="173"/>
+      <c r="X3" s="174"/>
     </row>
     <row r="4" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
@@ -3671,10 +3682,10 @@
     </row>
     <row r="15" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="120"/>
-      <c r="C15" s="175" t="s">
+      <c r="C15" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="176"/>
+      <c r="D15" s="168"/>
       <c r="E15" s="139">
         <f>AVERAGE(E5:E14)</f>
         <v>17.392159999999997</v>
@@ -3689,10 +3700,10 @@
         <v>71.8</v>
       </c>
       <c r="J15" s="120"/>
-      <c r="K15" s="175" t="s">
+      <c r="K15" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="176"/>
+      <c r="L15" s="168"/>
       <c r="M15" s="139">
         <f>AVERAGE(M5:M14)</f>
         <v>0.71133000000000002</v>
@@ -3707,10 +3718,10 @@
         <v>62.5</v>
       </c>
       <c r="R15" s="120"/>
-      <c r="S15" s="175" t="s">
+      <c r="S15" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="T15" s="176"/>
+      <c r="T15" s="168"/>
       <c r="U15" s="140">
         <f>AVERAGE(U5:U14)</f>
         <v>0.12404999999999999</v>
@@ -4377,10 +4388,10 @@
     </row>
     <row r="26" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="120"/>
-      <c r="C26" s="175" t="s">
+      <c r="C26" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="176"/>
+      <c r="D26" s="168"/>
       <c r="E26" s="140">
         <f>AVERAGE(E16:E25)</f>
         <v>44785.458460000002</v>
@@ -4395,10 +4406,10 @@
         <v>75.900000000000006</v>
       </c>
       <c r="J26" s="120"/>
-      <c r="K26" s="175" t="s">
+      <c r="K26" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="176"/>
+      <c r="L26" s="168"/>
       <c r="M26" s="140">
         <f>AVERAGE(M16:M25)</f>
         <v>1.0383599999999999</v>
@@ -4413,10 +4424,10 @@
         <v>76.7</v>
       </c>
       <c r="R26" s="120"/>
-      <c r="S26" s="175" t="s">
+      <c r="S26" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="176"/>
+      <c r="T26" s="168"/>
       <c r="U26" s="140">
         <f>AVERAGE(U16:U25)</f>
         <v>0.28898000000000007</v>
@@ -5083,10 +5094,10 @@
     </row>
     <row r="37" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="120"/>
-      <c r="C37" s="175" t="s">
+      <c r="C37" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="176"/>
+      <c r="D37" s="168"/>
       <c r="E37" s="140">
         <f>AVERAGE(E27:E36)</f>
         <v>-1</v>
@@ -5101,10 +5112,10 @@
         <v>62.6</v>
       </c>
       <c r="J37" s="120"/>
-      <c r="K37" s="175" t="s">
+      <c r="K37" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="L37" s="176"/>
+      <c r="L37" s="168"/>
       <c r="M37" s="140">
         <f>AVERAGE(M27:M36)</f>
         <v>2.0703299999999998</v>
@@ -5119,10 +5130,10 @@
         <v>67.2</v>
       </c>
       <c r="R37" s="120"/>
-      <c r="S37" s="175" t="s">
+      <c r="S37" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="T37" s="176"/>
+      <c r="T37" s="168"/>
       <c r="U37" s="140">
         <f>AVERAGE(U27:U36)</f>
         <v>6.5949999999999995E-2</v>
@@ -5789,10 +5800,10 @@
     </row>
     <row r="48" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="120"/>
-      <c r="C48" s="175" t="s">
+      <c r="C48" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="176"/>
+      <c r="D48" s="168"/>
       <c r="E48" s="140">
         <f>AVERAGE(E38:E47)</f>
         <v>-1</v>
@@ -5807,10 +5818,10 @@
         <v>74.400000000000006</v>
       </c>
       <c r="J48" s="120"/>
-      <c r="K48" s="175" t="s">
+      <c r="K48" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="176"/>
+      <c r="L48" s="168"/>
       <c r="M48" s="140">
         <f>AVERAGE(M38:M47)</f>
         <v>3.8687499999999999</v>
@@ -5825,10 +5836,10 @@
         <v>69.900000000000006</v>
       </c>
       <c r="R48" s="120"/>
-      <c r="S48" s="175" t="s">
+      <c r="S48" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="T48" s="176"/>
+      <c r="T48" s="168"/>
       <c r="U48" s="140">
         <f>AVERAGE(U38:U47)</f>
         <v>0.19390999999999997</v>
@@ -6494,10 +6505,10 @@
       </c>
     </row>
     <row r="59" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="175" t="s">
+      <c r="C59" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="176"/>
+      <c r="D59" s="168"/>
       <c r="E59" s="140">
         <f>AVERAGE(E49:E58)</f>
         <v>-1</v>
@@ -6511,10 +6522,10 @@
         <f>AVERAGE(H49:H58)</f>
         <v>66.2</v>
       </c>
-      <c r="K59" s="175" t="s">
+      <c r="K59" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="L59" s="176"/>
+      <c r="L59" s="168"/>
       <c r="M59" s="140">
         <f>AVERAGE(M49:M58)</f>
         <v>10.25055</v>
@@ -6528,10 +6539,10 @@
         <f>AVERAGE(P49:P58)</f>
         <v>62.5</v>
       </c>
-      <c r="S59" s="175" t="s">
+      <c r="S59" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="T59" s="176"/>
+      <c r="T59" s="168"/>
       <c r="U59" s="140">
         <f>AVERAGE(U49:U58)</f>
         <v>0.25315000000000004</v>
@@ -6548,37 +6559,37 @@
     </row>
     <row r="61" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C62" s="160" t="s">
+      <c r="C62" s="175" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="161"/>
-      <c r="E62" s="161"/>
-      <c r="F62" s="162"/>
+      <c r="D62" s="176"/>
+      <c r="E62" s="176"/>
+      <c r="F62" s="177"/>
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="C63" s="163"/>
-      <c r="D63" s="164"/>
-      <c r="E63" s="164"/>
-      <c r="F63" s="165"/>
+      <c r="C63" s="178"/>
+      <c r="D63" s="179"/>
+      <c r="E63" s="179"/>
+      <c r="F63" s="180"/>
     </row>
     <row r="64" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="166"/>
-      <c r="D64" s="167"/>
-      <c r="E64" s="167"/>
-      <c r="F64" s="168"/>
+      <c r="C64" s="181"/>
+      <c r="D64" s="182"/>
+      <c r="E64" s="182"/>
+      <c r="F64" s="183"/>
     </row>
     <row r="65" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="3:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="169" t="s">
+      <c r="C66" s="184" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="170"/>
-      <c r="E66" s="171"/>
+      <c r="D66" s="185"/>
+      <c r="E66" s="186"/>
     </row>
     <row r="67" spans="3:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="172"/>
-      <c r="D67" s="173"/>
-      <c r="E67" s="174"/>
+      <c r="C67" s="187"/>
+      <c r="D67" s="188"/>
+      <c r="E67" s="189"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C68" s="81" t="s">
@@ -6638,22 +6649,15 @@
     </row>
     <row r="74" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="180" t="s">
+      <c r="C75" s="164" t="s">
         <v>22</v>
       </c>
-      <c r="D75" s="181"/>
-      <c r="E75" s="181"/>
-      <c r="F75" s="182"/>
+      <c r="D75" s="165"/>
+      <c r="E75" s="165"/>
+      <c r="F75" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="S59:T59"/>
     <mergeCell ref="S2:X3"/>
     <mergeCell ref="C2:H3"/>
     <mergeCell ref="C62:F64"/>
@@ -6668,6 +6672,13 @@
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="K48:L48"/>
     <mergeCell ref="K2:P3"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="S59:T59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6679,7 +6690,7 @@
   <dimension ref="A2:K57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A2" sqref="A2:K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8500,7 +8511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074BBD8A-C58A-6D43-AB50-6FAB8ACE68BE}">
   <dimension ref="C1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -8508,25 +8519,25 @@
   <sheetData>
     <row r="1" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="186" t="b">
+      <c r="C2" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="185" t="s">
+      <c r="D2" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="191"/>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="191"/>
-      <c r="K2" s="191"/>
-      <c r="L2" s="191"/>
-      <c r="M2" s="192"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="163"/>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C3" s="187"/>
-      <c r="D3" s="188" t="s">
+      <c r="C3" s="158"/>
+      <c r="D3" s="159" t="s">
         <v>59</v>
       </c>
       <c r="E3" s="151"/>
@@ -8537,10 +8548,10 @@
       <c r="J3" s="151"/>
       <c r="K3" s="151"/>
       <c r="L3" s="151"/>
-      <c r="M3" s="184"/>
+      <c r="M3" s="155"/>
     </row>
     <row r="4" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="187"/>
+      <c r="C4" s="158"/>
       <c r="D4" s="151"/>
       <c r="E4" s="151"/>
       <c r="F4" s="151"/>
@@ -8550,13 +8561,13 @@
       <c r="J4" s="151"/>
       <c r="K4" s="151"/>
       <c r="L4" s="151"/>
-      <c r="M4" s="184"/>
+      <c r="M4" s="155"/>
     </row>
     <row r="5" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="186" t="b">
+      <c r="C5" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="185" t="s">
+      <c r="D5" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="151"/>
@@ -8567,25 +8578,25 @@
       <c r="J5" s="151"/>
       <c r="K5" s="151"/>
       <c r="L5" s="151"/>
-      <c r="M5" s="184"/>
+      <c r="M5" s="155"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C6" s="187"/>
-      <c r="D6" s="188" t="s">
+      <c r="C6" s="158"/>
+      <c r="D6" s="159" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="188"/>
-      <c r="F6" s="188"/>
-      <c r="G6" s="188"/>
-      <c r="H6" s="188"/>
-      <c r="I6" s="188"/>
-      <c r="J6" s="188"/>
-      <c r="K6" s="188"/>
+      <c r="E6" s="159"/>
+      <c r="F6" s="159"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="159"/>
+      <c r="I6" s="159"/>
+      <c r="J6" s="159"/>
+      <c r="K6" s="159"/>
       <c r="L6" s="151"/>
-      <c r="M6" s="184"/>
+      <c r="M6" s="155"/>
     </row>
     <row r="7" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="187"/>
+      <c r="C7" s="158"/>
       <c r="D7" s="151"/>
       <c r="E7" s="151"/>
       <c r="F7" s="151"/>
@@ -8595,13 +8606,13 @@
       <c r="J7" s="151"/>
       <c r="K7" s="151"/>
       <c r="L7" s="151"/>
-      <c r="M7" s="184"/>
+      <c r="M7" s="155"/>
     </row>
     <row r="8" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="186" t="b">
+      <c r="C8" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="185" t="s">
+      <c r="D8" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="151"/>
@@ -8612,25 +8623,25 @@
       <c r="J8" s="151"/>
       <c r="K8" s="151"/>
       <c r="L8" s="151"/>
-      <c r="M8" s="184"/>
+      <c r="M8" s="155"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C9" s="187"/>
-      <c r="D9" s="188" t="s">
+      <c r="C9" s="158"/>
+      <c r="D9" s="159" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="188"/>
-      <c r="F9" s="188"/>
-      <c r="G9" s="188"/>
-      <c r="H9" s="188"/>
-      <c r="I9" s="188"/>
-      <c r="J9" s="188"/>
-      <c r="K9" s="188"/>
+      <c r="E9" s="159"/>
+      <c r="F9" s="159"/>
+      <c r="G9" s="159"/>
+      <c r="H9" s="159"/>
+      <c r="I9" s="159"/>
+      <c r="J9" s="159"/>
+      <c r="K9" s="159"/>
       <c r="L9" s="151"/>
-      <c r="M9" s="184"/>
+      <c r="M9" s="155"/>
     </row>
     <row r="10" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="187"/>
+      <c r="C10" s="158"/>
       <c r="D10" s="151"/>
       <c r="E10" s="151"/>
       <c r="F10" s="151"/>
@@ -8640,13 +8651,13 @@
       <c r="J10" s="151"/>
       <c r="K10" s="151"/>
       <c r="L10" s="151"/>
-      <c r="M10" s="184"/>
+      <c r="M10" s="155"/>
     </row>
     <row r="11" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="186" t="b">
+      <c r="C11" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D11" s="185" t="s">
+      <c r="D11" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="151"/>
@@ -8657,11 +8668,11 @@
       <c r="J11" s="151"/>
       <c r="K11" s="151"/>
       <c r="L11" s="151"/>
-      <c r="M11" s="184"/>
+      <c r="M11" s="155"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C12" s="187"/>
-      <c r="D12" s="188" t="s">
+      <c r="C12" s="158"/>
+      <c r="D12" s="159" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="151"/>
@@ -8672,10 +8683,10 @@
       <c r="J12" s="151"/>
       <c r="K12" s="151"/>
       <c r="L12" s="151"/>
-      <c r="M12" s="184"/>
+      <c r="M12" s="155"/>
     </row>
     <row r="13" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="187"/>
+      <c r="C13" s="158"/>
       <c r="D13" s="151"/>
       <c r="E13" s="151"/>
       <c r="F13" s="151"/>
@@ -8685,13 +8696,13 @@
       <c r="J13" s="151"/>
       <c r="K13" s="151"/>
       <c r="L13" s="151"/>
-      <c r="M13" s="184"/>
+      <c r="M13" s="155"/>
     </row>
     <row r="14" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="186" t="b">
+      <c r="C14" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="185" t="s">
+      <c r="D14" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="151"/>
@@ -8702,10 +8713,10 @@
       <c r="J14" s="151"/>
       <c r="K14" s="151"/>
       <c r="L14" s="151"/>
-      <c r="M14" s="184"/>
+      <c r="M14" s="155"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C15" s="187"/>
+      <c r="C15" s="158"/>
       <c r="D15" s="151" t="s">
         <v>55</v>
       </c>
@@ -8717,10 +8728,10 @@
       <c r="J15" s="151"/>
       <c r="K15" s="151"/>
       <c r="L15" s="151"/>
-      <c r="M15" s="184"/>
+      <c r="M15" s="155"/>
     </row>
     <row r="16" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="187"/>
+      <c r="C16" s="158"/>
       <c r="D16" s="151"/>
       <c r="E16" s="151"/>
       <c r="F16" s="151"/>
@@ -8730,13 +8741,13 @@
       <c r="J16" s="151"/>
       <c r="K16" s="151"/>
       <c r="L16" s="151"/>
-      <c r="M16" s="184"/>
+      <c r="M16" s="155"/>
     </row>
     <row r="17" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="186" t="b">
+      <c r="C17" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="185" t="s">
+      <c r="D17" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="151"/>
@@ -8747,10 +8758,10 @@
       <c r="J17" s="151"/>
       <c r="K17" s="151"/>
       <c r="L17" s="151"/>
-      <c r="M17" s="184"/>
+      <c r="M17" s="155"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C18" s="187"/>
+      <c r="C18" s="158"/>
       <c r="D18" s="151" t="s">
         <v>54</v>
       </c>
@@ -8762,10 +8773,10 @@
       <c r="J18" s="151"/>
       <c r="K18" s="151"/>
       <c r="L18" s="151"/>
-      <c r="M18" s="184"/>
+      <c r="M18" s="155"/>
     </row>
     <row r="19" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="187"/>
+      <c r="C19" s="158"/>
       <c r="D19" s="151"/>
       <c r="E19" s="151"/>
       <c r="F19" s="151"/>
@@ -8775,13 +8786,13 @@
       <c r="J19" s="151"/>
       <c r="K19" s="151"/>
       <c r="L19" s="151"/>
-      <c r="M19" s="184"/>
+      <c r="M19" s="155"/>
     </row>
     <row r="20" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="186" t="b">
+      <c r="C20" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D20" s="185" t="s">
+      <c r="D20" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E20" s="151"/>
@@ -8792,10 +8803,10 @@
       <c r="J20" s="151"/>
       <c r="K20" s="151"/>
       <c r="L20" s="151"/>
-      <c r="M20" s="184"/>
+      <c r="M20" s="155"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C21" s="187"/>
+      <c r="C21" s="158"/>
       <c r="D21" s="151" t="s">
         <v>53</v>
       </c>
@@ -8807,10 +8818,10 @@
       <c r="J21" s="151"/>
       <c r="K21" s="151"/>
       <c r="L21" s="151"/>
-      <c r="M21" s="184"/>
+      <c r="M21" s="155"/>
     </row>
     <row r="22" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="187"/>
+      <c r="C22" s="158"/>
       <c r="D22" s="151"/>
       <c r="E22" s="151"/>
       <c r="F22" s="151"/>
@@ -8820,13 +8831,13 @@
       <c r="J22" s="151"/>
       <c r="K22" s="151"/>
       <c r="L22" s="151"/>
-      <c r="M22" s="184"/>
+      <c r="M22" s="155"/>
     </row>
     <row r="23" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="186" t="b">
+      <c r="C23" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="185" t="s">
+      <c r="D23" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="151"/>
@@ -8837,10 +8848,10 @@
       <c r="J23" s="151"/>
       <c r="K23" s="151"/>
       <c r="L23" s="151"/>
-      <c r="M23" s="184"/>
+      <c r="M23" s="155"/>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C24" s="187"/>
+      <c r="C24" s="158"/>
       <c r="D24" s="151" t="s">
         <v>52</v>
       </c>
@@ -8852,10 +8863,10 @@
       <c r="J24" s="151"/>
       <c r="K24" s="151"/>
       <c r="L24" s="151"/>
-      <c r="M24" s="184"/>
+      <c r="M24" s="155"/>
     </row>
     <row r="25" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="187"/>
+      <c r="C25" s="158"/>
       <c r="D25" s="151"/>
       <c r="E25" s="151"/>
       <c r="F25" s="151"/>
@@ -8865,13 +8876,13 @@
       <c r="J25" s="151"/>
       <c r="K25" s="151"/>
       <c r="L25" s="151"/>
-      <c r="M25" s="184"/>
+      <c r="M25" s="155"/>
     </row>
     <row r="26" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="186" t="b">
+      <c r="C26" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="185" t="s">
+      <c r="D26" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E26" s="151"/>
@@ -8882,10 +8893,10 @@
       <c r="J26" s="151"/>
       <c r="K26" s="151"/>
       <c r="L26" s="151"/>
-      <c r="M26" s="184"/>
+      <c r="M26" s="155"/>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C27" s="187"/>
+      <c r="C27" s="158"/>
       <c r="D27" s="151" t="s">
         <v>51</v>
       </c>
@@ -8897,10 +8908,10 @@
       <c r="J27" s="151"/>
       <c r="K27" s="151"/>
       <c r="L27" s="151"/>
-      <c r="M27" s="184"/>
+      <c r="M27" s="155"/>
     </row>
     <row r="28" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="187"/>
+      <c r="C28" s="158"/>
       <c r="D28" s="151"/>
       <c r="E28" s="151"/>
       <c r="F28" s="151"/>
@@ -8910,13 +8921,13 @@
       <c r="J28" s="151"/>
       <c r="K28" s="151"/>
       <c r="L28" s="151"/>
-      <c r="M28" s="184"/>
+      <c r="M28" s="155"/>
     </row>
     <row r="29" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="186" t="b">
+      <c r="C29" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D29" s="185" t="s">
+      <c r="D29" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="151"/>
@@ -8927,10 +8938,10 @@
       <c r="J29" s="151"/>
       <c r="K29" s="151"/>
       <c r="L29" s="151"/>
-      <c r="M29" s="184"/>
+      <c r="M29" s="155"/>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C30" s="187"/>
+      <c r="C30" s="158"/>
       <c r="D30" s="151" t="s">
         <v>50</v>
       </c>
@@ -8942,10 +8953,10 @@
       <c r="J30" s="151"/>
       <c r="K30" s="151"/>
       <c r="L30" s="151"/>
-      <c r="M30" s="184"/>
+      <c r="M30" s="155"/>
     </row>
     <row r="31" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="187"/>
+      <c r="C31" s="158"/>
       <c r="D31" s="151"/>
       <c r="E31" s="151"/>
       <c r="F31" s="151"/>
@@ -8955,13 +8966,13 @@
       <c r="J31" s="151"/>
       <c r="K31" s="151"/>
       <c r="L31" s="151"/>
-      <c r="M31" s="184"/>
+      <c r="M31" s="155"/>
     </row>
     <row r="32" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="186" t="b">
+      <c r="C32" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D32" s="185" t="s">
+      <c r="D32" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="151"/>
@@ -8972,10 +8983,10 @@
       <c r="J32" s="151"/>
       <c r="K32" s="151"/>
       <c r="L32" s="151"/>
-      <c r="M32" s="184"/>
+      <c r="M32" s="155"/>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C33" s="187"/>
+      <c r="C33" s="158"/>
       <c r="D33" s="151" t="s">
         <v>49</v>
       </c>
@@ -8987,10 +8998,10 @@
       <c r="J33" s="151"/>
       <c r="K33" s="151"/>
       <c r="L33" s="151"/>
-      <c r="M33" s="184"/>
+      <c r="M33" s="155"/>
     </row>
     <row r="34" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="187"/>
+      <c r="C34" s="158"/>
       <c r="D34" s="151"/>
       <c r="E34" s="151"/>
       <c r="F34" s="151"/>
@@ -9000,13 +9011,13 @@
       <c r="J34" s="151"/>
       <c r="K34" s="151"/>
       <c r="L34" s="151"/>
-      <c r="M34" s="184"/>
+      <c r="M34" s="155"/>
     </row>
     <row r="35" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="186" t="b">
+      <c r="C35" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D35" s="185" t="s">
+      <c r="D35" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E35" s="151"/>
@@ -9017,10 +9028,10 @@
       <c r="J35" s="151"/>
       <c r="K35" s="151"/>
       <c r="L35" s="151"/>
-      <c r="M35" s="184"/>
+      <c r="M35" s="155"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C36" s="187"/>
+      <c r="C36" s="158"/>
       <c r="D36" s="151" t="s">
         <v>48</v>
       </c>
@@ -9032,10 +9043,10 @@
       <c r="J36" s="151"/>
       <c r="K36" s="151"/>
       <c r="L36" s="151"/>
-      <c r="M36" s="184"/>
+      <c r="M36" s="155"/>
     </row>
     <row r="37" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="187"/>
+      <c r="C37" s="158"/>
       <c r="D37" s="151"/>
       <c r="E37" s="151"/>
       <c r="F37" s="151"/>
@@ -9045,13 +9056,13 @@
       <c r="J37" s="151"/>
       <c r="K37" s="151"/>
       <c r="L37" s="151"/>
-      <c r="M37" s="184"/>
+      <c r="M37" s="155"/>
     </row>
     <row r="38" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="186" t="b">
+      <c r="C38" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D38" s="185" t="s">
+      <c r="D38" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E38" s="151"/>
@@ -9062,10 +9073,10 @@
       <c r="J38" s="151"/>
       <c r="K38" s="151"/>
       <c r="L38" s="151"/>
-      <c r="M38" s="184"/>
+      <c r="M38" s="155"/>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C39" s="187"/>
+      <c r="C39" s="158"/>
       <c r="D39" s="151" t="s">
         <v>47</v>
       </c>
@@ -9077,10 +9088,10 @@
       <c r="J39" s="151"/>
       <c r="K39" s="151"/>
       <c r="L39" s="151"/>
-      <c r="M39" s="184"/>
+      <c r="M39" s="155"/>
     </row>
     <row r="40" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="187"/>
+      <c r="C40" s="158"/>
       <c r="D40" s="151"/>
       <c r="E40" s="151"/>
       <c r="F40" s="151"/>
@@ -9090,13 +9101,13 @@
       <c r="J40" s="151"/>
       <c r="K40" s="151"/>
       <c r="L40" s="151"/>
-      <c r="M40" s="184"/>
+      <c r="M40" s="155"/>
     </row>
     <row r="41" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="186" t="b">
+      <c r="C41" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D41" s="185" t="s">
+      <c r="D41" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="151"/>
@@ -9107,10 +9118,10 @@
       <c r="J41" s="151"/>
       <c r="K41" s="151"/>
       <c r="L41" s="151"/>
-      <c r="M41" s="184"/>
+      <c r="M41" s="155"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C42" s="187"/>
+      <c r="C42" s="158"/>
       <c r="D42" s="151" t="s">
         <v>46</v>
       </c>
@@ -9122,10 +9133,10 @@
       <c r="J42" s="151"/>
       <c r="K42" s="151"/>
       <c r="L42" s="151"/>
-      <c r="M42" s="184"/>
+      <c r="M42" s="155"/>
     </row>
     <row r="43" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="187"/>
+      <c r="C43" s="158"/>
       <c r="D43" s="151"/>
       <c r="E43" s="151"/>
       <c r="F43" s="151"/>
@@ -9135,13 +9146,13 @@
       <c r="J43" s="151"/>
       <c r="K43" s="151"/>
       <c r="L43" s="151"/>
-      <c r="M43" s="184"/>
+      <c r="M43" s="155"/>
     </row>
     <row r="44" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="186" t="b">
+      <c r="C44" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D44" s="185" t="s">
+      <c r="D44" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E44" s="151"/>
@@ -9152,10 +9163,10 @@
       <c r="J44" s="151"/>
       <c r="K44" s="151"/>
       <c r="L44" s="151"/>
-      <c r="M44" s="184"/>
+      <c r="M44" s="155"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C45" s="187"/>
+      <c r="C45" s="158"/>
       <c r="D45" s="151" t="s">
         <v>45</v>
       </c>
@@ -9167,10 +9178,10 @@
       <c r="J45" s="151"/>
       <c r="K45" s="151"/>
       <c r="L45" s="151"/>
-      <c r="M45" s="184"/>
+      <c r="M45" s="155"/>
     </row>
     <row r="46" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="187"/>
+      <c r="C46" s="158"/>
       <c r="D46" s="151"/>
       <c r="E46" s="151"/>
       <c r="F46" s="151"/>
@@ -9180,13 +9191,13 @@
       <c r="J46" s="151"/>
       <c r="K46" s="151"/>
       <c r="L46" s="151"/>
-      <c r="M46" s="184"/>
+      <c r="M46" s="155"/>
     </row>
     <row r="47" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="186" t="b">
+      <c r="C47" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D47" s="185" t="s">
+      <c r="D47" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E47" s="151"/>
@@ -9197,10 +9208,10 @@
       <c r="J47" s="151"/>
       <c r="K47" s="151"/>
       <c r="L47" s="151"/>
-      <c r="M47" s="184"/>
+      <c r="M47" s="155"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C48" s="187"/>
+      <c r="C48" s="158"/>
       <c r="D48" s="151" t="s">
         <v>44</v>
       </c>
@@ -9212,10 +9223,10 @@
       <c r="J48" s="151"/>
       <c r="K48" s="151"/>
       <c r="L48" s="151"/>
-      <c r="M48" s="184"/>
+      <c r="M48" s="155"/>
     </row>
     <row r="49" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="187"/>
+      <c r="C49" s="158"/>
       <c r="D49" s="151"/>
       <c r="E49" s="151"/>
       <c r="F49" s="151"/>
@@ -9225,13 +9236,13 @@
       <c r="J49" s="151"/>
       <c r="K49" s="151"/>
       <c r="L49" s="151"/>
-      <c r="M49" s="184"/>
+      <c r="M49" s="155"/>
     </row>
     <row r="50" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="186" t="b">
+      <c r="C50" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D50" s="185" t="s">
+      <c r="D50" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E50" s="151"/>
@@ -9242,10 +9253,10 @@
       <c r="J50" s="151"/>
       <c r="K50" s="151"/>
       <c r="L50" s="151"/>
-      <c r="M50" s="184"/>
+      <c r="M50" s="155"/>
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C51" s="187"/>
+      <c r="C51" s="158"/>
       <c r="D51" s="151" t="s">
         <v>43</v>
       </c>
@@ -9257,10 +9268,10 @@
       <c r="J51" s="151"/>
       <c r="K51" s="151"/>
       <c r="L51" s="151"/>
-      <c r="M51" s="184"/>
+      <c r="M51" s="155"/>
     </row>
     <row r="52" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="187"/>
+      <c r="C52" s="158"/>
       <c r="D52" s="151"/>
       <c r="E52" s="151"/>
       <c r="F52" s="151"/>
@@ -9270,13 +9281,13 @@
       <c r="J52" s="151"/>
       <c r="K52" s="151"/>
       <c r="L52" s="151"/>
-      <c r="M52" s="184"/>
+      <c r="M52" s="155"/>
     </row>
     <row r="53" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="186" t="b">
+      <c r="C53" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D53" s="185" t="s">
+      <c r="D53" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E53" s="151"/>
@@ -9287,10 +9298,10 @@
       <c r="J53" s="151"/>
       <c r="K53" s="151"/>
       <c r="L53" s="151"/>
-      <c r="M53" s="184"/>
+      <c r="M53" s="155"/>
     </row>
     <row r="54" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C54" s="187"/>
+      <c r="C54" s="158"/>
       <c r="D54" s="151" t="s">
         <v>42</v>
       </c>
@@ -9302,10 +9313,10 @@
       <c r="J54" s="151"/>
       <c r="K54" s="151"/>
       <c r="L54" s="151"/>
-      <c r="M54" s="184"/>
+      <c r="M54" s="155"/>
     </row>
     <row r="55" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="187"/>
+      <c r="C55" s="158"/>
       <c r="D55" s="151"/>
       <c r="E55" s="151"/>
       <c r="F55" s="151"/>
@@ -9315,13 +9326,13 @@
       <c r="J55" s="151"/>
       <c r="K55" s="151"/>
       <c r="L55" s="151"/>
-      <c r="M55" s="184"/>
+      <c r="M55" s="155"/>
     </row>
     <row r="56" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="186" t="b">
+      <c r="C56" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D56" s="185" t="s">
+      <c r="D56" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E56" s="151"/>
@@ -9332,10 +9343,10 @@
       <c r="J56" s="151"/>
       <c r="K56" s="151"/>
       <c r="L56" s="151"/>
-      <c r="M56" s="184"/>
+      <c r="M56" s="155"/>
     </row>
     <row r="57" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C57" s="187"/>
+      <c r="C57" s="158"/>
       <c r="D57" s="151" t="s">
         <v>41</v>
       </c>
@@ -9347,10 +9358,10 @@
       <c r="J57" s="151"/>
       <c r="K57" s="151"/>
       <c r="L57" s="151"/>
-      <c r="M57" s="184"/>
+      <c r="M57" s="155"/>
     </row>
     <row r="58" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="187"/>
+      <c r="C58" s="158"/>
       <c r="D58" s="151"/>
       <c r="E58" s="151"/>
       <c r="F58" s="151"/>
@@ -9360,13 +9371,13 @@
       <c r="J58" s="151"/>
       <c r="K58" s="151"/>
       <c r="L58" s="151"/>
-      <c r="M58" s="184"/>
+      <c r="M58" s="155"/>
     </row>
     <row r="59" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="186" t="b">
+      <c r="C59" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D59" s="185" t="s">
+      <c r="D59" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E59" s="151"/>
@@ -9377,10 +9388,10 @@
       <c r="J59" s="151"/>
       <c r="K59" s="151"/>
       <c r="L59" s="151"/>
-      <c r="M59" s="184"/>
+      <c r="M59" s="155"/>
     </row>
     <row r="60" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C60" s="187"/>
+      <c r="C60" s="158"/>
       <c r="D60" s="151" t="s">
         <v>40</v>
       </c>
@@ -9392,10 +9403,10 @@
       <c r="J60" s="151"/>
       <c r="K60" s="151"/>
       <c r="L60" s="151"/>
-      <c r="M60" s="184"/>
+      <c r="M60" s="155"/>
     </row>
     <row r="61" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="187"/>
+      <c r="C61" s="158"/>
       <c r="D61" s="151"/>
       <c r="E61" s="151"/>
       <c r="F61" s="151"/>
@@ -9405,13 +9416,13 @@
       <c r="J61" s="151"/>
       <c r="K61" s="151"/>
       <c r="L61" s="151"/>
-      <c r="M61" s="184"/>
+      <c r="M61" s="155"/>
     </row>
     <row r="62" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C62" s="186" t="b">
+      <c r="C62" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D62" s="185" t="s">
+      <c r="D62" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E62" s="151"/>
@@ -9422,10 +9433,10 @@
       <c r="J62" s="151"/>
       <c r="K62" s="151"/>
       <c r="L62" s="151"/>
-      <c r="M62" s="184"/>
+      <c r="M62" s="155"/>
     </row>
     <row r="63" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C63" s="187"/>
+      <c r="C63" s="158"/>
       <c r="D63" s="151" t="s">
         <v>39</v>
       </c>
@@ -9437,10 +9448,10 @@
       <c r="J63" s="151"/>
       <c r="K63" s="151"/>
       <c r="L63" s="151"/>
-      <c r="M63" s="184"/>
+      <c r="M63" s="155"/>
     </row>
     <row r="64" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="187"/>
+      <c r="C64" s="158"/>
       <c r="D64" s="151"/>
       <c r="E64" s="151"/>
       <c r="F64" s="151"/>
@@ -9450,13 +9461,13 @@
       <c r="J64" s="151"/>
       <c r="K64" s="151"/>
       <c r="L64" s="151"/>
-      <c r="M64" s="184"/>
+      <c r="M64" s="155"/>
     </row>
     <row r="65" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="186" t="b">
+      <c r="C65" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D65" s="185" t="s">
+      <c r="D65" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E65" s="151"/>
@@ -9467,10 +9478,10 @@
       <c r="J65" s="151"/>
       <c r="K65" s="151"/>
       <c r="L65" s="151"/>
-      <c r="M65" s="184"/>
+      <c r="M65" s="155"/>
     </row>
     <row r="66" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C66" s="187"/>
+      <c r="C66" s="158"/>
       <c r="D66" s="151" t="s">
         <v>38</v>
       </c>
@@ -9482,10 +9493,10 @@
       <c r="J66" s="151"/>
       <c r="K66" s="151"/>
       <c r="L66" s="151"/>
-      <c r="M66" s="184"/>
+      <c r="M66" s="155"/>
     </row>
     <row r="67" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="187"/>
+      <c r="C67" s="158"/>
       <c r="D67" s="151"/>
       <c r="E67" s="151"/>
       <c r="F67" s="151"/>
@@ -9495,13 +9506,13 @@
       <c r="J67" s="151"/>
       <c r="K67" s="151"/>
       <c r="L67" s="151"/>
-      <c r="M67" s="184"/>
+      <c r="M67" s="155"/>
     </row>
     <row r="68" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="186" t="b">
+      <c r="C68" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D68" s="185" t="s">
+      <c r="D68" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E68" s="151"/>
@@ -9512,10 +9523,10 @@
       <c r="J68" s="151"/>
       <c r="K68" s="151"/>
       <c r="L68" s="151"/>
-      <c r="M68" s="184"/>
+      <c r="M68" s="155"/>
     </row>
     <row r="69" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C69" s="187"/>
+      <c r="C69" s="158"/>
       <c r="D69" s="151" t="s">
         <v>37</v>
       </c>
@@ -9527,10 +9538,10 @@
       <c r="J69" s="151"/>
       <c r="K69" s="151"/>
       <c r="L69" s="151"/>
-      <c r="M69" s="184"/>
+      <c r="M69" s="155"/>
     </row>
     <row r="70" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="187"/>
+      <c r="C70" s="158"/>
       <c r="D70" s="151"/>
       <c r="E70" s="151"/>
       <c r="F70" s="151"/>
@@ -9540,13 +9551,13 @@
       <c r="J70" s="151"/>
       <c r="K70" s="151"/>
       <c r="L70" s="151"/>
-      <c r="M70" s="184"/>
+      <c r="M70" s="155"/>
     </row>
     <row r="71" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C71" s="186" t="b">
+      <c r="C71" s="157" t="b">
         <v>1</v>
       </c>
-      <c r="D71" s="185" t="s">
+      <c r="D71" s="156" t="s">
         <v>36</v>
       </c>
       <c r="E71" s="151"/>
@@ -9557,22 +9568,22 @@
       <c r="J71" s="151"/>
       <c r="K71" s="151"/>
       <c r="L71" s="151"/>
-      <c r="M71" s="184"/>
+      <c r="M71" s="155"/>
     </row>
     <row r="72" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="183"/>
-      <c r="D72" s="189" t="s">
+      <c r="C72" s="154"/>
+      <c r="D72" s="160" t="s">
         <v>35</v>
       </c>
-      <c r="E72" s="189"/>
-      <c r="F72" s="189"/>
-      <c r="G72" s="189"/>
-      <c r="H72" s="189"/>
-      <c r="I72" s="189"/>
-      <c r="J72" s="189"/>
-      <c r="K72" s="189"/>
-      <c r="L72" s="189"/>
-      <c r="M72" s="190"/>
+      <c r="E72" s="160"/>
+      <c r="F72" s="160"/>
+      <c r="G72" s="160"/>
+      <c r="H72" s="160"/>
+      <c r="I72" s="160"/>
+      <c r="J72" s="160"/>
+      <c r="K72" s="160"/>
+      <c r="L72" s="160"/>
+      <c r="M72" s="161"/>
     </row>
     <row r="73" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C73" s="151"/>
@@ -9777,56 +9788,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="formula" val="TRUE"/>
-        <cfvo type="formula" val="FALSE"/>
-        <color theme="9"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="formula" val="TRUE"/>
-        <cfvo type="formula" val="FALSE"/>
-        <color theme="9"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="formula" val="TRUE"/>
-        <cfvo type="formula" val="FALSE"/>
-        <color theme="9"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="formula" val="TRUE"/>
-        <cfvo type="formula" val="FALSE"/>
-        <color theme="9"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="formula" val="TRUE"/>
-        <cfvo type="formula" val="FALSE"/>
-        <color theme="9"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D41">
     <cfRule type="colorScale" priority="6">
       <colorScale>
@@ -9887,6 +9848,1891 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="formula" val="TRUE"/>
+        <cfvo type="formula" val="FALSE"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97A1125-9A1C-7543-8DFB-66461D641281}">
+  <dimension ref="A1:N51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="153" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="153" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="151">
+        <v>1</v>
+      </c>
+      <c r="B2" s="143">
+        <v>0.49969999999999998</v>
+      </c>
+      <c r="C2" s="152">
+        <v>65</v>
+      </c>
+      <c r="D2" s="147">
+        <v>191</v>
+      </c>
+      <c r="E2" s="145">
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="F2" s="152">
+        <v>65</v>
+      </c>
+      <c r="G2" s="147">
+        <v>191</v>
+      </c>
+      <c r="H2" s="149">
+        <v>11.975199999999999</v>
+      </c>
+      <c r="I2" s="152">
+        <v>65</v>
+      </c>
+      <c r="J2" s="147">
+        <v>191</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="193">
+        <f>MEDIAN(H2:H11)</f>
+        <v>8.2458500000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="151">
+        <v>2</v>
+      </c>
+      <c r="B3" s="143">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="C3" s="152">
+        <v>74</v>
+      </c>
+      <c r="D3" s="147">
+        <v>206</v>
+      </c>
+      <c r="E3" s="142">
+        <v>0.77939999999999998</v>
+      </c>
+      <c r="F3" s="152">
+        <v>74</v>
+      </c>
+      <c r="G3" s="147">
+        <v>206</v>
+      </c>
+      <c r="H3" s="149">
+        <v>8.2377000000000002</v>
+      </c>
+      <c r="I3" s="152">
+        <v>74</v>
+      </c>
+      <c r="J3" s="147">
+        <v>206</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="193">
+        <f>MEDIAN(B2:B11)</f>
+        <v>3.6049999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="151">
+        <v>3</v>
+      </c>
+      <c r="B4" s="143">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="C4" s="152">
+        <v>44</v>
+      </c>
+      <c r="D4" s="147">
+        <v>132</v>
+      </c>
+      <c r="E4" s="143">
+        <v>9.9599999999999994E-2</v>
+      </c>
+      <c r="F4" s="152">
+        <v>44</v>
+      </c>
+      <c r="G4" s="147">
+        <v>132</v>
+      </c>
+      <c r="H4" s="149">
+        <v>0.20069999999999999</v>
+      </c>
+      <c r="I4" s="152">
+        <v>44</v>
+      </c>
+      <c r="J4" s="147">
+        <v>132</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="193">
+        <f>MEDIAN(E2:E11)</f>
+        <v>0.33550000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="151">
+        <v>4</v>
+      </c>
+      <c r="B5" s="143">
+        <v>3.73E-2</v>
+      </c>
+      <c r="C5" s="152">
+        <v>74</v>
+      </c>
+      <c r="D5" s="147">
+        <v>206</v>
+      </c>
+      <c r="E5" s="143">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="F5" s="152">
+        <v>74</v>
+      </c>
+      <c r="G5" s="147">
+        <v>206</v>
+      </c>
+      <c r="H5" s="149">
+        <v>8.2539999999999996</v>
+      </c>
+      <c r="I5" s="152">
+        <v>74</v>
+      </c>
+      <c r="J5" s="147">
+        <v>206</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="151">
+        <v>5</v>
+      </c>
+      <c r="B6" s="143">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="C6" s="152">
+        <v>47</v>
+      </c>
+      <c r="D6" s="147">
+        <v>141</v>
+      </c>
+      <c r="E6" s="143">
+        <v>0.11310000000000001</v>
+      </c>
+      <c r="F6" s="152">
+        <v>47</v>
+      </c>
+      <c r="G6" s="147">
+        <v>141</v>
+      </c>
+      <c r="H6" s="149">
+        <v>0.30759999999999998</v>
+      </c>
+      <c r="I6" s="152">
+        <v>47</v>
+      </c>
+      <c r="J6" s="147">
+        <v>141</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="151">
+        <v>6</v>
+      </c>
+      <c r="B7" s="143">
+        <v>0.48359999999999997</v>
+      </c>
+      <c r="C7" s="152">
+        <v>116</v>
+      </c>
+      <c r="D7" s="147">
+        <v>281</v>
+      </c>
+      <c r="E7" s="143">
+        <v>2.0668000000000002</v>
+      </c>
+      <c r="F7" s="152">
+        <v>84</v>
+      </c>
+      <c r="G7" s="147">
+        <v>219</v>
+      </c>
+      <c r="H7" s="149">
+        <v>22.0045</v>
+      </c>
+      <c r="I7" s="152">
+        <v>89</v>
+      </c>
+      <c r="J7" s="147">
+        <v>227</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="151">
+        <v>7</v>
+      </c>
+      <c r="B8" s="143">
+        <v>2.58E-2</v>
+      </c>
+      <c r="C8" s="152">
+        <v>65</v>
+      </c>
+      <c r="D8" s="147">
+        <v>182</v>
+      </c>
+      <c r="E8" s="143">
+        <v>7.0199999999999999E-2</v>
+      </c>
+      <c r="F8" s="152">
+        <v>23</v>
+      </c>
+      <c r="G8" s="147">
+        <v>78</v>
+      </c>
+      <c r="H8" s="149">
+        <v>0.46260000000000001</v>
+      </c>
+      <c r="I8" s="152">
+        <v>64</v>
+      </c>
+      <c r="J8" s="147">
+        <v>180</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="151">
+        <v>8</v>
+      </c>
+      <c r="B9" s="143">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C9" s="152">
+        <v>100</v>
+      </c>
+      <c r="D9" s="147">
+        <v>248</v>
+      </c>
+      <c r="E9" s="143">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="F9" s="152">
+        <v>36</v>
+      </c>
+      <c r="G9" s="147">
+        <v>111</v>
+      </c>
+      <c r="H9" s="150">
+        <v>106.7842</v>
+      </c>
+      <c r="I9" s="152">
+        <v>119</v>
+      </c>
+      <c r="J9" s="147">
+        <v>284</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="151">
+        <v>9</v>
+      </c>
+      <c r="B10" s="143">
+        <v>0.03</v>
+      </c>
+      <c r="C10" s="152">
+        <v>84</v>
+      </c>
+      <c r="D10" s="147">
+        <v>219</v>
+      </c>
+      <c r="E10" s="143">
+        <v>0.47410000000000002</v>
+      </c>
+      <c r="F10" s="152">
+        <v>76</v>
+      </c>
+      <c r="G10" s="147">
+        <v>201</v>
+      </c>
+      <c r="H10" s="150">
+        <v>15.649100000000001</v>
+      </c>
+      <c r="I10" s="152">
+        <v>98</v>
+      </c>
+      <c r="J10" s="147">
+        <v>245</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="151">
+        <v>10</v>
+      </c>
+      <c r="B11" s="143">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="C11" s="152">
+        <v>36</v>
+      </c>
+      <c r="D11" s="147">
+        <v>111</v>
+      </c>
+      <c r="E11" s="143">
+        <v>0.55269999999999997</v>
+      </c>
+      <c r="F11" s="152">
+        <v>102</v>
+      </c>
+      <c r="G11" s="147">
+        <v>253</v>
+      </c>
+      <c r="H11" s="150">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I11" s="152">
+        <v>44</v>
+      </c>
+      <c r="J11" s="147">
+        <v>134</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="151">
+        <v>11</v>
+      </c>
+      <c r="B12" s="143">
+        <v>1.5162</v>
+      </c>
+      <c r="C12" s="152">
+        <v>84</v>
+      </c>
+      <c r="D12" s="147">
+        <v>345</v>
+      </c>
+      <c r="E12" s="143">
+        <v>2.7269999999999999</v>
+      </c>
+      <c r="F12" s="152">
+        <v>84</v>
+      </c>
+      <c r="G12" s="147">
+        <v>345</v>
+      </c>
+      <c r="H12" s="149">
+        <v>6679.2203</v>
+      </c>
+      <c r="I12" s="152">
+        <v>84</v>
+      </c>
+      <c r="J12" s="147">
+        <v>345</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="151">
+        <v>12</v>
+      </c>
+      <c r="B13" s="143">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="C13" s="152">
+        <v>65</v>
+      </c>
+      <c r="D13" s="147">
+        <v>281</v>
+      </c>
+      <c r="E13" s="143">
+        <v>0.49740000000000001</v>
+      </c>
+      <c r="F13" s="152">
+        <v>65</v>
+      </c>
+      <c r="G13" s="147">
+        <v>281</v>
+      </c>
+      <c r="H13" s="149">
+        <v>276.4384</v>
+      </c>
+      <c r="I13" s="152">
+        <v>65</v>
+      </c>
+      <c r="J13" s="147">
+        <v>281</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="151">
+        <v>13</v>
+      </c>
+      <c r="B14" s="143">
+        <v>0.12790000000000001</v>
+      </c>
+      <c r="C14" s="152">
+        <v>92</v>
+      </c>
+      <c r="D14" s="147">
+        <v>368</v>
+      </c>
+      <c r="E14" s="143">
+        <v>1.0585</v>
+      </c>
+      <c r="F14" s="152">
+        <v>92</v>
+      </c>
+      <c r="G14" s="147">
+        <v>368</v>
+      </c>
+      <c r="H14" s="149">
+        <v>22679.67</v>
+      </c>
+      <c r="I14" s="152">
+        <v>92</v>
+      </c>
+      <c r="J14" s="147">
+        <v>368</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="151">
+        <v>14</v>
+      </c>
+      <c r="B15" s="143">
+        <v>0.2147</v>
+      </c>
+      <c r="C15" s="152">
+        <v>84</v>
+      </c>
+      <c r="D15" s="147">
+        <v>345</v>
+      </c>
+      <c r="E15" s="143">
+        <v>0.68969999999999998</v>
+      </c>
+      <c r="F15" s="152">
+        <v>84</v>
+      </c>
+      <c r="G15" s="147">
+        <v>345</v>
+      </c>
+      <c r="H15" s="149">
+        <v>6668.933</v>
+      </c>
+      <c r="I15" s="152">
+        <v>84</v>
+      </c>
+      <c r="J15" s="147">
+        <v>345</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="151">
+        <v>15</v>
+      </c>
+      <c r="B16" s="143">
+        <v>0.25130000000000002</v>
+      </c>
+      <c r="C16" s="152">
+        <v>110</v>
+      </c>
+      <c r="D16" s="147">
+        <v>416</v>
+      </c>
+      <c r="E16" s="143">
+        <v>1.0362</v>
+      </c>
+      <c r="F16" s="152">
+        <v>110</v>
+      </c>
+      <c r="G16" s="147">
+        <v>416</v>
+      </c>
+      <c r="H16" s="149">
+        <v>310926.12319999997</v>
+      </c>
+      <c r="I16" s="152">
+        <v>110</v>
+      </c>
+      <c r="J16" s="147">
+        <v>416</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="151">
+        <v>16</v>
+      </c>
+      <c r="B17" s="143">
+        <v>0.60870000000000002</v>
+      </c>
+      <c r="C17" s="152">
+        <v>78</v>
+      </c>
+      <c r="D17" s="147">
+        <v>314</v>
+      </c>
+      <c r="E17" s="143">
+        <v>2.1147999999999998</v>
+      </c>
+      <c r="F17" s="152">
+        <v>99</v>
+      </c>
+      <c r="G17" s="147">
+        <v>373</v>
+      </c>
+      <c r="H17" s="150">
+        <v>85928.341400000005</v>
+      </c>
+      <c r="I17" s="152">
+        <v>113</v>
+      </c>
+      <c r="J17" s="147">
+        <v>410</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="151">
+        <v>17</v>
+      </c>
+      <c r="B18" s="143">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="C18" s="152">
+        <v>44</v>
+      </c>
+      <c r="D18" s="147">
+        <v>207</v>
+      </c>
+      <c r="E18" s="143">
+        <v>0.1668</v>
+      </c>
+      <c r="F18" s="152">
+        <v>23</v>
+      </c>
+      <c r="G18" s="147">
+        <v>110</v>
+      </c>
+      <c r="H18" s="150">
+        <v>5.9802</v>
+      </c>
+      <c r="I18" s="152">
+        <v>51</v>
+      </c>
+      <c r="J18" s="147">
+        <v>231</v>
+      </c>
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="151">
+        <v>18</v>
+      </c>
+      <c r="B19" s="143">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="C19" s="152">
+        <v>41</v>
+      </c>
+      <c r="D19" s="147">
+        <v>189</v>
+      </c>
+      <c r="E19" s="143">
+        <v>0.1762</v>
+      </c>
+      <c r="F19" s="152">
+        <v>23</v>
+      </c>
+      <c r="G19" s="147">
+        <v>110</v>
+      </c>
+      <c r="H19" s="150">
+        <v>0.19370000000000001</v>
+      </c>
+      <c r="I19" s="152">
+        <v>33</v>
+      </c>
+      <c r="J19" s="147">
+        <v>159</v>
+      </c>
+      <c r="K19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="151">
+        <v>19</v>
+      </c>
+      <c r="B20" s="143">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="C20" s="152">
+        <v>111</v>
+      </c>
+      <c r="D20" s="147">
+        <v>403</v>
+      </c>
+      <c r="E20" s="143">
+        <v>1.5837000000000001</v>
+      </c>
+      <c r="F20" s="152">
+        <v>103</v>
+      </c>
+      <c r="G20" s="147">
+        <v>384</v>
+      </c>
+      <c r="H20" s="150">
+        <v>6.0100000000000001E-2</v>
+      </c>
+      <c r="I20" s="152">
+        <v>27</v>
+      </c>
+      <c r="J20" s="147">
+        <v>140</v>
+      </c>
+      <c r="K20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="151">
+        <v>20</v>
+      </c>
+      <c r="B21" s="143">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="C21" s="152">
+        <v>73</v>
+      </c>
+      <c r="D21" s="147">
+        <v>297</v>
+      </c>
+      <c r="E21" s="143">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F21" s="152">
+        <v>84</v>
+      </c>
+      <c r="G21" s="147">
+        <v>331</v>
+      </c>
+      <c r="H21" s="150">
+        <v>14689.624299999999</v>
+      </c>
+      <c r="I21" s="152">
+        <v>100</v>
+      </c>
+      <c r="J21" s="147">
+        <v>375</v>
+      </c>
+      <c r="K21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="151">
+        <v>21</v>
+      </c>
+      <c r="B22" s="143">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="C22" s="152">
+        <v>62</v>
+      </c>
+      <c r="D22" s="147">
+        <v>309</v>
+      </c>
+      <c r="E22" s="143">
+        <v>4.9534000000000002</v>
+      </c>
+      <c r="F22" s="152">
+        <v>62</v>
+      </c>
+      <c r="G22" s="147">
+        <v>309</v>
+      </c>
+      <c r="H22" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I22" s="147">
+        <v>0</v>
+      </c>
+      <c r="J22" s="147">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="151">
+        <v>22</v>
+      </c>
+      <c r="B23" s="143">
+        <v>6.6799999999999998E-2</v>
+      </c>
+      <c r="C23" s="152">
+        <v>47</v>
+      </c>
+      <c r="D23" s="147">
+        <v>241</v>
+      </c>
+      <c r="E23" s="143">
+        <v>0.65559999999999996</v>
+      </c>
+      <c r="F23" s="152">
+        <v>47</v>
+      </c>
+      <c r="G23" s="147">
+        <v>241</v>
+      </c>
+      <c r="H23" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I23" s="147">
+        <v>0</v>
+      </c>
+      <c r="J23" s="147">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="151">
+        <v>23</v>
+      </c>
+      <c r="B24" s="143">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C24" s="152">
+        <v>47</v>
+      </c>
+      <c r="D24" s="147">
+        <v>241</v>
+      </c>
+      <c r="E24" s="143">
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="F24" s="152">
+        <v>47</v>
+      </c>
+      <c r="G24" s="147">
+        <v>241</v>
+      </c>
+      <c r="H24" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I24" s="147">
+        <v>0</v>
+      </c>
+      <c r="J24" s="147">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="151">
+        <v>24</v>
+      </c>
+      <c r="B25" s="143">
+        <v>9.5699999999999993E-2</v>
+      </c>
+      <c r="C25" s="152">
+        <v>62</v>
+      </c>
+      <c r="D25" s="147">
+        <v>309</v>
+      </c>
+      <c r="E25" s="143">
+        <v>0.9294</v>
+      </c>
+      <c r="F25" s="152">
+        <v>62</v>
+      </c>
+      <c r="G25" s="147">
+        <v>309</v>
+      </c>
+      <c r="H25" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I25" s="147">
+        <v>0</v>
+      </c>
+      <c r="J25" s="147">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="151">
+        <v>25</v>
+      </c>
+      <c r="B26" s="143">
+        <v>0.1081</v>
+      </c>
+      <c r="C26" s="152">
+        <v>65</v>
+      </c>
+      <c r="D26" s="147">
+        <v>323</v>
+      </c>
+      <c r="E26" s="143">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="F26" s="152">
+        <v>65</v>
+      </c>
+      <c r="G26" s="147">
+        <v>323</v>
+      </c>
+      <c r="H26" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I26" s="147">
+        <v>0</v>
+      </c>
+      <c r="J26" s="147">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="151">
+        <v>26</v>
+      </c>
+      <c r="B27" s="143">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="C27" s="152">
+        <v>29</v>
+      </c>
+      <c r="D27" s="147">
+        <v>141</v>
+      </c>
+      <c r="E27" s="143">
+        <v>1.6797</v>
+      </c>
+      <c r="F27" s="152">
+        <v>49</v>
+      </c>
+      <c r="G27" s="147">
+        <v>231</v>
+      </c>
+      <c r="H27" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I27" s="147">
+        <v>0</v>
+      </c>
+      <c r="J27" s="147">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="151">
+        <v>27</v>
+      </c>
+      <c r="B28" s="143">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="C28" s="152">
+        <v>28</v>
+      </c>
+      <c r="D28" s="147">
+        <v>139</v>
+      </c>
+      <c r="E28" s="143">
+        <v>1.7325999999999999</v>
+      </c>
+      <c r="F28" s="152">
+        <v>53</v>
+      </c>
+      <c r="G28" s="147">
+        <v>243</v>
+      </c>
+      <c r="H28" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I28" s="147">
+        <v>0</v>
+      </c>
+      <c r="J28" s="147">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="151">
+        <v>28</v>
+      </c>
+      <c r="B29" s="143">
+        <v>4.6899999999999997E-2</v>
+      </c>
+      <c r="C29" s="152">
+        <v>49</v>
+      </c>
+      <c r="D29" s="147">
+        <v>231</v>
+      </c>
+      <c r="E29" s="143">
+        <v>4.1151</v>
+      </c>
+      <c r="F29" s="152">
+        <v>97</v>
+      </c>
+      <c r="G29" s="147">
+        <v>403</v>
+      </c>
+      <c r="H29" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I29" s="147">
+        <v>0</v>
+      </c>
+      <c r="J29" s="147">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="151">
+        <v>29</v>
+      </c>
+      <c r="B30" s="143">
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="C30" s="152">
+        <v>57</v>
+      </c>
+      <c r="D30" s="147">
+        <v>258</v>
+      </c>
+      <c r="E30" s="143">
+        <v>3.8875000000000002</v>
+      </c>
+      <c r="F30" s="152">
+        <v>95</v>
+      </c>
+      <c r="G30" s="147">
+        <v>394</v>
+      </c>
+      <c r="H30" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I30" s="147">
+        <v>0</v>
+      </c>
+      <c r="J30" s="147">
+        <v>0</v>
+      </c>
+      <c r="K30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="151">
+        <v>30</v>
+      </c>
+      <c r="B31" s="143">
+        <v>2.6800000000000001E-2</v>
+      </c>
+      <c r="C31" s="152">
+        <v>29</v>
+      </c>
+      <c r="D31" s="147">
+        <v>141</v>
+      </c>
+      <c r="E31" s="143">
+        <v>1.0582</v>
+      </c>
+      <c r="F31" s="152">
+        <v>95</v>
+      </c>
+      <c r="G31" s="147">
+        <v>394</v>
+      </c>
+      <c r="H31" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I31" s="147">
+        <v>0</v>
+      </c>
+      <c r="J31" s="147">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="151">
+        <v>31</v>
+      </c>
+      <c r="B32" s="143">
+        <v>0.126</v>
+      </c>
+      <c r="C32" s="152">
+        <v>44</v>
+      </c>
+      <c r="D32" s="147">
+        <v>220</v>
+      </c>
+      <c r="E32" s="143">
+        <v>5.3082000000000003</v>
+      </c>
+      <c r="F32" s="152">
+        <v>44</v>
+      </c>
+      <c r="G32" s="147">
+        <v>220</v>
+      </c>
+      <c r="H32" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I32" s="147">
+        <v>0</v>
+      </c>
+      <c r="J32" s="147">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="151">
+        <v>32</v>
+      </c>
+      <c r="B33" s="143">
+        <v>0.24690000000000001</v>
+      </c>
+      <c r="C33" s="152">
+        <v>110</v>
+      </c>
+      <c r="D33" s="147">
+        <v>469</v>
+      </c>
+      <c r="E33" s="143">
+        <v>5.5472999999999999</v>
+      </c>
+      <c r="F33" s="152">
+        <v>110</v>
+      </c>
+      <c r="G33" s="147">
+        <v>469</v>
+      </c>
+      <c r="H33" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I33" s="147">
+        <v>0</v>
+      </c>
+      <c r="J33" s="147">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="151">
+        <v>33</v>
+      </c>
+      <c r="B34" s="143">
+        <v>0.28860000000000002</v>
+      </c>
+      <c r="C34" s="152">
+        <v>87</v>
+      </c>
+      <c r="D34" s="147">
+        <v>389</v>
+      </c>
+      <c r="E34" s="143">
+        <v>3.3715999999999999</v>
+      </c>
+      <c r="F34" s="152">
+        <v>87</v>
+      </c>
+      <c r="G34" s="147">
+        <v>389</v>
+      </c>
+      <c r="H34" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I34" s="147">
+        <v>0</v>
+      </c>
+      <c r="J34" s="147">
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="151">
+        <v>34</v>
+      </c>
+      <c r="B35" s="143">
+        <v>0.22209999999999999</v>
+      </c>
+      <c r="C35" s="152">
+        <v>74</v>
+      </c>
+      <c r="D35" s="147">
+        <v>339</v>
+      </c>
+      <c r="E35" s="143">
+        <v>2.6358999999999999</v>
+      </c>
+      <c r="F35" s="152">
+        <v>74</v>
+      </c>
+      <c r="G35" s="147">
+        <v>339</v>
+      </c>
+      <c r="H35" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I35" s="147">
+        <v>0</v>
+      </c>
+      <c r="J35" s="147">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="151">
+        <v>35</v>
+      </c>
+      <c r="B36" s="143">
+        <v>0.35149999999999998</v>
+      </c>
+      <c r="C36" s="152">
+        <v>65</v>
+      </c>
+      <c r="D36" s="147">
+        <v>305</v>
+      </c>
+      <c r="E36" s="143">
+        <v>2.1475</v>
+      </c>
+      <c r="F36" s="152">
+        <v>65</v>
+      </c>
+      <c r="G36" s="147">
+        <v>305</v>
+      </c>
+      <c r="H36" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I36" s="147">
+        <v>0</v>
+      </c>
+      <c r="J36" s="147">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="151">
+        <v>36</v>
+      </c>
+      <c r="B37" s="143">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C37" s="152">
+        <v>110</v>
+      </c>
+      <c r="D37" s="147">
+        <v>548</v>
+      </c>
+      <c r="E37" s="143">
+        <v>1.4863999999999999</v>
+      </c>
+      <c r="F37" s="152">
+        <v>29</v>
+      </c>
+      <c r="G37" s="147">
+        <v>146</v>
+      </c>
+      <c r="H37" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I37" s="147">
+        <v>0</v>
+      </c>
+      <c r="J37" s="147">
+        <v>0</v>
+      </c>
+      <c r="K37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="151">
+        <v>37</v>
+      </c>
+      <c r="B38" s="143">
+        <v>0.15670000000000001</v>
+      </c>
+      <c r="C38" s="152">
+        <v>113</v>
+      </c>
+      <c r="D38" s="147">
+        <v>564</v>
+      </c>
+      <c r="E38" s="143">
+        <v>8.6432000000000002</v>
+      </c>
+      <c r="F38" s="152">
+        <v>101</v>
+      </c>
+      <c r="G38" s="147">
+        <v>511</v>
+      </c>
+      <c r="H38" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I38" s="147">
+        <v>0</v>
+      </c>
+      <c r="J38" s="147">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="151">
+        <v>38</v>
+      </c>
+      <c r="B39" s="143">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="C39" s="152">
+        <v>38</v>
+      </c>
+      <c r="D39" s="147">
+        <v>216</v>
+      </c>
+      <c r="E39" s="143">
+        <v>6.0906000000000002</v>
+      </c>
+      <c r="F39" s="152">
+        <v>76</v>
+      </c>
+      <c r="G39" s="147">
+        <v>402</v>
+      </c>
+      <c r="H39" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I39" s="147">
+        <v>0</v>
+      </c>
+      <c r="J39" s="147">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="151">
+        <v>39</v>
+      </c>
+      <c r="B40" s="143">
+        <v>0.13170000000000001</v>
+      </c>
+      <c r="C40" s="152">
+        <v>89</v>
+      </c>
+      <c r="D40" s="147">
+        <v>457</v>
+      </c>
+      <c r="E40" s="143">
+        <v>1.6453</v>
+      </c>
+      <c r="F40" s="152">
+        <v>33</v>
+      </c>
+      <c r="G40" s="147">
+        <v>181</v>
+      </c>
+      <c r="H40" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I40" s="147">
+        <v>0</v>
+      </c>
+      <c r="J40" s="147">
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="151">
+        <v>40</v>
+      </c>
+      <c r="B41" s="143">
+        <v>0.18909999999999999</v>
+      </c>
+      <c r="C41" s="152">
+        <v>118</v>
+      </c>
+      <c r="D41" s="147">
+        <v>582</v>
+      </c>
+      <c r="E41" s="143">
+        <v>1.8115000000000001</v>
+      </c>
+      <c r="F41" s="152">
+        <v>80</v>
+      </c>
+      <c r="G41" s="147">
+        <v>419</v>
+      </c>
+      <c r="H41" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I41" s="147">
+        <v>0</v>
+      </c>
+      <c r="J41" s="147">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="151">
+        <v>41</v>
+      </c>
+      <c r="B42" s="143">
+        <v>0.22850000000000001</v>
+      </c>
+      <c r="C42" s="152">
+        <v>47</v>
+      </c>
+      <c r="D42" s="147">
+        <v>255</v>
+      </c>
+      <c r="E42" s="143">
+        <v>12.73</v>
+      </c>
+      <c r="F42" s="152">
+        <v>47</v>
+      </c>
+      <c r="G42" s="147">
+        <v>255</v>
+      </c>
+      <c r="H42" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I42" s="147">
+        <v>0</v>
+      </c>
+      <c r="J42" s="147">
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="151">
+        <v>42</v>
+      </c>
+      <c r="B43" s="143">
+        <v>0.34789999999999999</v>
+      </c>
+      <c r="C43" s="152">
+        <v>84</v>
+      </c>
+      <c r="D43" s="147">
+        <v>440</v>
+      </c>
+      <c r="E43" s="143">
+        <v>9.5709</v>
+      </c>
+      <c r="F43" s="152">
+        <v>84</v>
+      </c>
+      <c r="G43" s="147">
+        <v>440</v>
+      </c>
+      <c r="H43" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I43" s="147">
+        <v>0</v>
+      </c>
+      <c r="J43" s="147">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="151">
+        <v>43</v>
+      </c>
+      <c r="B44" s="143">
+        <v>0.2127</v>
+      </c>
+      <c r="C44" s="152">
+        <v>44</v>
+      </c>
+      <c r="D44" s="147">
+        <v>238</v>
+      </c>
+      <c r="E44" s="143">
+        <v>2.4516</v>
+      </c>
+      <c r="F44" s="152">
+        <v>44</v>
+      </c>
+      <c r="G44" s="147">
+        <v>238</v>
+      </c>
+      <c r="H44" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I44" s="147">
+        <v>0</v>
+      </c>
+      <c r="J44" s="147">
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="151">
+        <v>44</v>
+      </c>
+      <c r="B45" s="143">
+        <v>0.43869999999999998</v>
+      </c>
+      <c r="C45" s="152">
+        <v>92</v>
+      </c>
+      <c r="D45" s="147">
+        <v>481</v>
+      </c>
+      <c r="E45" s="143">
+        <v>8.1262000000000008</v>
+      </c>
+      <c r="F45" s="152">
+        <v>92</v>
+      </c>
+      <c r="G45" s="147">
+        <v>481</v>
+      </c>
+      <c r="H45" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I45" s="147">
+        <v>0</v>
+      </c>
+      <c r="J45" s="147">
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="151">
+        <v>45</v>
+      </c>
+      <c r="B46" s="143">
+        <v>0.35449999999999998</v>
+      </c>
+      <c r="C46" s="152">
+        <v>74</v>
+      </c>
+      <c r="D46" s="147">
+        <v>393</v>
+      </c>
+      <c r="E46" s="143">
+        <v>5.8920000000000003</v>
+      </c>
+      <c r="F46" s="152">
+        <v>74</v>
+      </c>
+      <c r="G46" s="147">
+        <v>393</v>
+      </c>
+      <c r="H46" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I46" s="147">
+        <v>0</v>
+      </c>
+      <c r="J46" s="147">
+        <v>0</v>
+      </c>
+      <c r="K46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="151">
+        <v>46</v>
+      </c>
+      <c r="B47" s="143">
+        <v>0.24030000000000001</v>
+      </c>
+      <c r="C47" s="152">
+        <v>74</v>
+      </c>
+      <c r="D47" s="147">
+        <v>376</v>
+      </c>
+      <c r="E47" s="143">
+        <v>48.258499999999998</v>
+      </c>
+      <c r="F47" s="152">
+        <v>110</v>
+      </c>
+      <c r="G47" s="147">
+        <v>537</v>
+      </c>
+      <c r="H47" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I47" s="147">
+        <v>0</v>
+      </c>
+      <c r="J47" s="147">
+        <v>0</v>
+      </c>
+      <c r="K47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="151">
+        <v>47</v>
+      </c>
+      <c r="B48" s="143">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="C48" s="152">
+        <v>68</v>
+      </c>
+      <c r="D48" s="147">
+        <v>347</v>
+      </c>
+      <c r="E48" s="143">
+        <v>4.1337000000000002</v>
+      </c>
+      <c r="F48" s="152">
+        <v>36</v>
+      </c>
+      <c r="G48" s="147">
+        <v>198</v>
+      </c>
+      <c r="H48" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I48" s="147">
+        <v>0</v>
+      </c>
+      <c r="J48" s="147">
+        <v>0</v>
+      </c>
+      <c r="K48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="151">
+        <v>48</v>
+      </c>
+      <c r="B49" s="143">
+        <v>0.1797</v>
+      </c>
+      <c r="C49" s="152">
+        <v>57</v>
+      </c>
+      <c r="D49" s="147">
+        <v>300</v>
+      </c>
+      <c r="E49" s="143">
+        <v>2.7877000000000001</v>
+      </c>
+      <c r="F49" s="152">
+        <v>29</v>
+      </c>
+      <c r="G49" s="147">
+        <v>146</v>
+      </c>
+      <c r="H49" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I49" s="147">
+        <v>0</v>
+      </c>
+      <c r="J49" s="147">
+        <v>0</v>
+      </c>
+      <c r="K49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="151">
+        <v>49</v>
+      </c>
+      <c r="B50" s="143">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="C50" s="152">
+        <v>99</v>
+      </c>
+      <c r="D50" s="147">
+        <v>490</v>
+      </c>
+      <c r="E50" s="143">
+        <v>5.6365999999999996</v>
+      </c>
+      <c r="F50" s="152">
+        <v>44</v>
+      </c>
+      <c r="G50" s="147">
+        <v>239</v>
+      </c>
+      <c r="H50" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I50" s="147">
+        <v>0</v>
+      </c>
+      <c r="J50" s="147">
+        <v>0</v>
+      </c>
+      <c r="K50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="151">
+        <v>50</v>
+      </c>
+      <c r="B51" s="143">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="C51" s="152">
+        <v>22</v>
+      </c>
+      <c r="D51" s="147">
+        <v>110</v>
+      </c>
+      <c r="E51" s="143">
+        <v>2.9182999999999999</v>
+      </c>
+      <c r="F51" s="152">
+        <v>65</v>
+      </c>
+      <c r="G51" s="147">
+        <v>336</v>
+      </c>
+      <c r="H51" s="149">
+        <v>-1</v>
+      </c>
+      <c r="I51" s="147">
+        <v>0</v>
+      </c>
+      <c r="J51" s="147">
+        <v>0</v>
+      </c>
+      <c r="K51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes and performance improvements + added stopwatch
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbalkovec/Desktop/CPSC4100/FinalProject/FinalProject4100/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4C1D16-138D-AE42-91CA-BDD9FBEA04CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB3CF1A-2177-5E40-ADD1-711D1464F0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" activeTab="4" xr2:uid="{DE1357BD-E7FA-854A-BAD7-FAF24432C206}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" activeTab="3" xr2:uid="{DE1357BD-E7FA-854A-BAD7-FAF24432C206}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual" sheetId="1" r:id="rId1"/>
     <sheet name="Raw" sheetId="2" r:id="rId2"/>
     <sheet name="Unit Tests" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Estimates" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="69">
   <si>
     <t>Recursive</t>
   </si>
@@ -10047,1820 +10046,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97A1125-9A1C-7543-8DFB-66461D641281}">
-  <dimension ref="A1:K51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="M2:N4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="153" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="153" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="151">
-        <v>1</v>
-      </c>
-      <c r="B2" s="143">
-        <v>0.49969999999999998</v>
-      </c>
-      <c r="C2" s="152">
-        <v>65</v>
-      </c>
-      <c r="D2" s="147">
-        <v>191</v>
-      </c>
-      <c r="E2" s="145">
-        <v>2.6160000000000001</v>
-      </c>
-      <c r="F2" s="152">
-        <v>65</v>
-      </c>
-      <c r="G2" s="147">
-        <v>191</v>
-      </c>
-      <c r="H2" s="149">
-        <v>11.975199999999999</v>
-      </c>
-      <c r="I2" s="152">
-        <v>65</v>
-      </c>
-      <c r="J2" s="147">
-        <v>191</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="151">
-        <v>2</v>
-      </c>
-      <c r="B3" s="143">
-        <v>4.0500000000000001E-2</v>
-      </c>
-      <c r="C3" s="152">
-        <v>74</v>
-      </c>
-      <c r="D3" s="147">
-        <v>206</v>
-      </c>
-      <c r="E3" s="142">
-        <v>0.77939999999999998</v>
-      </c>
-      <c r="F3" s="152">
-        <v>74</v>
-      </c>
-      <c r="G3" s="147">
-        <v>206</v>
-      </c>
-      <c r="H3" s="149">
-        <v>8.2377000000000002</v>
-      </c>
-      <c r="I3" s="152">
-        <v>74</v>
-      </c>
-      <c r="J3" s="147">
-        <v>206</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="151">
-        <v>3</v>
-      </c>
-      <c r="B4" s="143">
-        <v>3.1199999999999999E-2</v>
-      </c>
-      <c r="C4" s="152">
-        <v>44</v>
-      </c>
-      <c r="D4" s="147">
-        <v>132</v>
-      </c>
-      <c r="E4" s="143">
-        <v>9.9599999999999994E-2</v>
-      </c>
-      <c r="F4" s="152">
-        <v>44</v>
-      </c>
-      <c r="G4" s="147">
-        <v>132</v>
-      </c>
-      <c r="H4" s="149">
-        <v>0.20069999999999999</v>
-      </c>
-      <c r="I4" s="152">
-        <v>44</v>
-      </c>
-      <c r="J4" s="147">
-        <v>132</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="151">
-        <v>4</v>
-      </c>
-      <c r="B5" s="143">
-        <v>3.73E-2</v>
-      </c>
-      <c r="C5" s="152">
-        <v>74</v>
-      </c>
-      <c r="D5" s="147">
-        <v>206</v>
-      </c>
-      <c r="E5" s="143">
-        <v>0.19689999999999999</v>
-      </c>
-      <c r="F5" s="152">
-        <v>74</v>
-      </c>
-      <c r="G5" s="147">
-        <v>206</v>
-      </c>
-      <c r="H5" s="149">
-        <v>8.2539999999999996</v>
-      </c>
-      <c r="I5" s="152">
-        <v>74</v>
-      </c>
-      <c r="J5" s="147">
-        <v>206</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="151">
-        <v>5</v>
-      </c>
-      <c r="B6" s="143">
-        <v>3.7100000000000001E-2</v>
-      </c>
-      <c r="C6" s="152">
-        <v>47</v>
-      </c>
-      <c r="D6" s="147">
-        <v>141</v>
-      </c>
-      <c r="E6" s="143">
-        <v>0.11310000000000001</v>
-      </c>
-      <c r="F6" s="152">
-        <v>47</v>
-      </c>
-      <c r="G6" s="147">
-        <v>141</v>
-      </c>
-      <c r="H6" s="149">
-        <v>0.30759999999999998</v>
-      </c>
-      <c r="I6" s="152">
-        <v>47</v>
-      </c>
-      <c r="J6" s="147">
-        <v>141</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="151">
-        <v>6</v>
-      </c>
-      <c r="B7" s="143">
-        <v>0.48359999999999997</v>
-      </c>
-      <c r="C7" s="152">
-        <v>116</v>
-      </c>
-      <c r="D7" s="147">
-        <v>281</v>
-      </c>
-      <c r="E7" s="143">
-        <v>2.0668000000000002</v>
-      </c>
-      <c r="F7" s="152">
-        <v>84</v>
-      </c>
-      <c r="G7" s="147">
-        <v>219</v>
-      </c>
-      <c r="H7" s="149">
-        <v>22.0045</v>
-      </c>
-      <c r="I7" s="152">
-        <v>89</v>
-      </c>
-      <c r="J7" s="147">
-        <v>227</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="151">
-        <v>7</v>
-      </c>
-      <c r="B8" s="143">
-        <v>2.58E-2</v>
-      </c>
-      <c r="C8" s="152">
-        <v>65</v>
-      </c>
-      <c r="D8" s="147">
-        <v>182</v>
-      </c>
-      <c r="E8" s="143">
-        <v>7.0199999999999999E-2</v>
-      </c>
-      <c r="F8" s="152">
-        <v>23</v>
-      </c>
-      <c r="G8" s="147">
-        <v>78</v>
-      </c>
-      <c r="H8" s="149">
-        <v>0.46260000000000001</v>
-      </c>
-      <c r="I8" s="152">
-        <v>64</v>
-      </c>
-      <c r="J8" s="147">
-        <v>180</v>
-      </c>
-      <c r="K8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="151">
-        <v>8</v>
-      </c>
-      <c r="B9" s="143">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="C9" s="152">
-        <v>100</v>
-      </c>
-      <c r="D9" s="147">
-        <v>248</v>
-      </c>
-      <c r="E9" s="143">
-        <v>0.14449999999999999</v>
-      </c>
-      <c r="F9" s="152">
-        <v>36</v>
-      </c>
-      <c r="G9" s="147">
-        <v>111</v>
-      </c>
-      <c r="H9" s="150">
-        <v>106.7842</v>
-      </c>
-      <c r="I9" s="152">
-        <v>119</v>
-      </c>
-      <c r="J9" s="147">
-        <v>284</v>
-      </c>
-      <c r="K9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="151">
-        <v>9</v>
-      </c>
-      <c r="B10" s="143">
-        <v>0.03</v>
-      </c>
-      <c r="C10" s="152">
-        <v>84</v>
-      </c>
-      <c r="D10" s="147">
-        <v>219</v>
-      </c>
-      <c r="E10" s="143">
-        <v>0.47410000000000002</v>
-      </c>
-      <c r="F10" s="152">
-        <v>76</v>
-      </c>
-      <c r="G10" s="147">
-        <v>201</v>
-      </c>
-      <c r="H10" s="150">
-        <v>15.649100000000001</v>
-      </c>
-      <c r="I10" s="152">
-        <v>98</v>
-      </c>
-      <c r="J10" s="147">
-        <v>245</v>
-      </c>
-      <c r="K10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="151">
-        <v>10</v>
-      </c>
-      <c r="B11" s="143">
-        <v>2.0299999999999999E-2</v>
-      </c>
-      <c r="C11" s="152">
-        <v>36</v>
-      </c>
-      <c r="D11" s="147">
-        <v>111</v>
-      </c>
-      <c r="E11" s="143">
-        <v>0.55269999999999997</v>
-      </c>
-      <c r="F11" s="152">
-        <v>102</v>
-      </c>
-      <c r="G11" s="147">
-        <v>253</v>
-      </c>
-      <c r="H11" s="150">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="I11" s="152">
-        <v>44</v>
-      </c>
-      <c r="J11" s="147">
-        <v>134</v>
-      </c>
-      <c r="K11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="151">
-        <v>11</v>
-      </c>
-      <c r="B12" s="143">
-        <v>1.5162</v>
-      </c>
-      <c r="C12" s="152">
-        <v>84</v>
-      </c>
-      <c r="D12" s="147">
-        <v>345</v>
-      </c>
-      <c r="E12" s="143">
-        <v>2.7269999999999999</v>
-      </c>
-      <c r="F12" s="152">
-        <v>84</v>
-      </c>
-      <c r="G12" s="147">
-        <v>345</v>
-      </c>
-      <c r="H12" s="149">
-        <v>6679.2203</v>
-      </c>
-      <c r="I12" s="152">
-        <v>84</v>
-      </c>
-      <c r="J12" s="147">
-        <v>345</v>
-      </c>
-      <c r="K12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="151">
-        <v>12</v>
-      </c>
-      <c r="B13" s="143">
-        <v>5.2699999999999997E-2</v>
-      </c>
-      <c r="C13" s="152">
-        <v>65</v>
-      </c>
-      <c r="D13" s="147">
-        <v>281</v>
-      </c>
-      <c r="E13" s="143">
-        <v>0.49740000000000001</v>
-      </c>
-      <c r="F13" s="152">
-        <v>65</v>
-      </c>
-      <c r="G13" s="147">
-        <v>281</v>
-      </c>
-      <c r="H13" s="149">
-        <v>276.4384</v>
-      </c>
-      <c r="I13" s="152">
-        <v>65</v>
-      </c>
-      <c r="J13" s="147">
-        <v>281</v>
-      </c>
-      <c r="K13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="151">
-        <v>13</v>
-      </c>
-      <c r="B14" s="143">
-        <v>0.12790000000000001</v>
-      </c>
-      <c r="C14" s="152">
-        <v>92</v>
-      </c>
-      <c r="D14" s="147">
-        <v>368</v>
-      </c>
-      <c r="E14" s="143">
-        <v>1.0585</v>
-      </c>
-      <c r="F14" s="152">
-        <v>92</v>
-      </c>
-      <c r="G14" s="147">
-        <v>368</v>
-      </c>
-      <c r="H14" s="149">
-        <v>22679.67</v>
-      </c>
-      <c r="I14" s="152">
-        <v>92</v>
-      </c>
-      <c r="J14" s="147">
-        <v>368</v>
-      </c>
-      <c r="K14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="151">
-        <v>14</v>
-      </c>
-      <c r="B15" s="143">
-        <v>0.2147</v>
-      </c>
-      <c r="C15" s="152">
-        <v>84</v>
-      </c>
-      <c r="D15" s="147">
-        <v>345</v>
-      </c>
-      <c r="E15" s="143">
-        <v>0.68969999999999998</v>
-      </c>
-      <c r="F15" s="152">
-        <v>84</v>
-      </c>
-      <c r="G15" s="147">
-        <v>345</v>
-      </c>
-      <c r="H15" s="149">
-        <v>6668.933</v>
-      </c>
-      <c r="I15" s="152">
-        <v>84</v>
-      </c>
-      <c r="J15" s="147">
-        <v>345</v>
-      </c>
-      <c r="K15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="151">
-        <v>15</v>
-      </c>
-      <c r="B16" s="143">
-        <v>0.25130000000000002</v>
-      </c>
-      <c r="C16" s="152">
-        <v>110</v>
-      </c>
-      <c r="D16" s="147">
-        <v>416</v>
-      </c>
-      <c r="E16" s="143">
-        <v>1.0362</v>
-      </c>
-      <c r="F16" s="152">
-        <v>110</v>
-      </c>
-      <c r="G16" s="147">
-        <v>416</v>
-      </c>
-      <c r="H16" s="149">
-        <v>310926.12319999997</v>
-      </c>
-      <c r="I16" s="152">
-        <v>110</v>
-      </c>
-      <c r="J16" s="147">
-        <v>416</v>
-      </c>
-      <c r="K16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="151">
-        <v>16</v>
-      </c>
-      <c r="B17" s="143">
-        <v>0.60870000000000002</v>
-      </c>
-      <c r="C17" s="152">
-        <v>78</v>
-      </c>
-      <c r="D17" s="147">
-        <v>314</v>
-      </c>
-      <c r="E17" s="143">
-        <v>2.1147999999999998</v>
-      </c>
-      <c r="F17" s="152">
-        <v>99</v>
-      </c>
-      <c r="G17" s="147">
-        <v>373</v>
-      </c>
-      <c r="H17" s="150">
-        <v>85928.341400000005</v>
-      </c>
-      <c r="I17" s="152">
-        <v>113</v>
-      </c>
-      <c r="J17" s="147">
-        <v>410</v>
-      </c>
-      <c r="K17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="151">
-        <v>17</v>
-      </c>
-      <c r="B18" s="143">
-        <v>2.1399999999999999E-2</v>
-      </c>
-      <c r="C18" s="152">
-        <v>44</v>
-      </c>
-      <c r="D18" s="147">
-        <v>207</v>
-      </c>
-      <c r="E18" s="143">
-        <v>0.1668</v>
-      </c>
-      <c r="F18" s="152">
-        <v>23</v>
-      </c>
-      <c r="G18" s="147">
-        <v>110</v>
-      </c>
-      <c r="H18" s="150">
-        <v>5.9802</v>
-      </c>
-      <c r="I18" s="152">
-        <v>51</v>
-      </c>
-      <c r="J18" s="147">
-        <v>231</v>
-      </c>
-      <c r="K18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="151">
-        <v>18</v>
-      </c>
-      <c r="B19" s="143">
-        <v>2.2599999999999999E-2</v>
-      </c>
-      <c r="C19" s="152">
-        <v>41</v>
-      </c>
-      <c r="D19" s="147">
-        <v>189</v>
-      </c>
-      <c r="E19" s="143">
-        <v>0.1762</v>
-      </c>
-      <c r="F19" s="152">
-        <v>23</v>
-      </c>
-      <c r="G19" s="147">
-        <v>110</v>
-      </c>
-      <c r="H19" s="150">
-        <v>0.19370000000000001</v>
-      </c>
-      <c r="I19" s="152">
-        <v>33</v>
-      </c>
-      <c r="J19" s="147">
-        <v>159</v>
-      </c>
-      <c r="K19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="151">
-        <v>19</v>
-      </c>
-      <c r="B20" s="143">
-        <v>4.3499999999999997E-2</v>
-      </c>
-      <c r="C20" s="152">
-        <v>111</v>
-      </c>
-      <c r="D20" s="147">
-        <v>403</v>
-      </c>
-      <c r="E20" s="143">
-        <v>1.5837000000000001</v>
-      </c>
-      <c r="F20" s="152">
-        <v>103</v>
-      </c>
-      <c r="G20" s="147">
-        <v>384</v>
-      </c>
-      <c r="H20" s="150">
-        <v>6.0100000000000001E-2</v>
-      </c>
-      <c r="I20" s="152">
-        <v>27</v>
-      </c>
-      <c r="J20" s="147">
-        <v>140</v>
-      </c>
-      <c r="K20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="151">
-        <v>20</v>
-      </c>
-      <c r="B21" s="143">
-        <v>3.0800000000000001E-2</v>
-      </c>
-      <c r="C21" s="152">
-        <v>73</v>
-      </c>
-      <c r="D21" s="147">
-        <v>297</v>
-      </c>
-      <c r="E21" s="143">
-        <v>0.33329999999999999</v>
-      </c>
-      <c r="F21" s="152">
-        <v>84</v>
-      </c>
-      <c r="G21" s="147">
-        <v>331</v>
-      </c>
-      <c r="H21" s="150">
-        <v>14689.624299999999</v>
-      </c>
-      <c r="I21" s="152">
-        <v>100</v>
-      </c>
-      <c r="J21" s="147">
-        <v>375</v>
-      </c>
-      <c r="K21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="151">
-        <v>21</v>
-      </c>
-      <c r="B22" s="143">
-        <v>9.8500000000000004E-2</v>
-      </c>
-      <c r="C22" s="152">
-        <v>62</v>
-      </c>
-      <c r="D22" s="147">
-        <v>309</v>
-      </c>
-      <c r="E22" s="143">
-        <v>4.9534000000000002</v>
-      </c>
-      <c r="F22" s="152">
-        <v>62</v>
-      </c>
-      <c r="G22" s="147">
-        <v>309</v>
-      </c>
-      <c r="H22" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I22" s="147">
-        <v>0</v>
-      </c>
-      <c r="J22" s="147">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="151">
-        <v>22</v>
-      </c>
-      <c r="B23" s="143">
-        <v>6.6799999999999998E-2</v>
-      </c>
-      <c r="C23" s="152">
-        <v>47</v>
-      </c>
-      <c r="D23" s="147">
-        <v>241</v>
-      </c>
-      <c r="E23" s="143">
-        <v>0.65559999999999996</v>
-      </c>
-      <c r="F23" s="152">
-        <v>47</v>
-      </c>
-      <c r="G23" s="147">
-        <v>241</v>
-      </c>
-      <c r="H23" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I23" s="147">
-        <v>0</v>
-      </c>
-      <c r="J23" s="147">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="151">
-        <v>23</v>
-      </c>
-      <c r="B24" s="143">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="C24" s="152">
-        <v>47</v>
-      </c>
-      <c r="D24" s="147">
-        <v>241</v>
-      </c>
-      <c r="E24" s="143">
-        <v>0.70130000000000003</v>
-      </c>
-      <c r="F24" s="152">
-        <v>47</v>
-      </c>
-      <c r="G24" s="147">
-        <v>241</v>
-      </c>
-      <c r="H24" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I24" s="147">
-        <v>0</v>
-      </c>
-      <c r="J24" s="147">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="151">
-        <v>24</v>
-      </c>
-      <c r="B25" s="143">
-        <v>9.5699999999999993E-2</v>
-      </c>
-      <c r="C25" s="152">
-        <v>62</v>
-      </c>
-      <c r="D25" s="147">
-        <v>309</v>
-      </c>
-      <c r="E25" s="143">
-        <v>0.9294</v>
-      </c>
-      <c r="F25" s="152">
-        <v>62</v>
-      </c>
-      <c r="G25" s="147">
-        <v>309</v>
-      </c>
-      <c r="H25" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I25" s="147">
-        <v>0</v>
-      </c>
-      <c r="J25" s="147">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="151">
-        <v>25</v>
-      </c>
-      <c r="B26" s="143">
-        <v>0.1081</v>
-      </c>
-      <c r="C26" s="152">
-        <v>65</v>
-      </c>
-      <c r="D26" s="147">
-        <v>323</v>
-      </c>
-      <c r="E26" s="143">
-        <v>0.99050000000000005</v>
-      </c>
-      <c r="F26" s="152">
-        <v>65</v>
-      </c>
-      <c r="G26" s="147">
-        <v>323</v>
-      </c>
-      <c r="H26" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I26" s="147">
-        <v>0</v>
-      </c>
-      <c r="J26" s="147">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="151">
-        <v>26</v>
-      </c>
-      <c r="B27" s="143">
-        <v>3.0800000000000001E-2</v>
-      </c>
-      <c r="C27" s="152">
-        <v>29</v>
-      </c>
-      <c r="D27" s="147">
-        <v>141</v>
-      </c>
-      <c r="E27" s="143">
-        <v>1.6797</v>
-      </c>
-      <c r="F27" s="152">
-        <v>49</v>
-      </c>
-      <c r="G27" s="147">
-        <v>231</v>
-      </c>
-      <c r="H27" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I27" s="147">
-        <v>0</v>
-      </c>
-      <c r="J27" s="147">
-        <v>0</v>
-      </c>
-      <c r="K27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="151">
-        <v>27</v>
-      </c>
-      <c r="B28" s="143">
-        <v>2.9700000000000001E-2</v>
-      </c>
-      <c r="C28" s="152">
-        <v>28</v>
-      </c>
-      <c r="D28" s="147">
-        <v>139</v>
-      </c>
-      <c r="E28" s="143">
-        <v>1.7325999999999999</v>
-      </c>
-      <c r="F28" s="152">
-        <v>53</v>
-      </c>
-      <c r="G28" s="147">
-        <v>243</v>
-      </c>
-      <c r="H28" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I28" s="147">
-        <v>0</v>
-      </c>
-      <c r="J28" s="147">
-        <v>0</v>
-      </c>
-      <c r="K28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="151">
-        <v>28</v>
-      </c>
-      <c r="B29" s="143">
-        <v>4.6899999999999997E-2</v>
-      </c>
-      <c r="C29" s="152">
-        <v>49</v>
-      </c>
-      <c r="D29" s="147">
-        <v>231</v>
-      </c>
-      <c r="E29" s="143">
-        <v>4.1151</v>
-      </c>
-      <c r="F29" s="152">
-        <v>97</v>
-      </c>
-      <c r="G29" s="147">
-        <v>403</v>
-      </c>
-      <c r="H29" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I29" s="147">
-        <v>0</v>
-      </c>
-      <c r="J29" s="147">
-        <v>0</v>
-      </c>
-      <c r="K29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="151">
-        <v>29</v>
-      </c>
-      <c r="B30" s="143">
-        <v>6.1199999999999997E-2</v>
-      </c>
-      <c r="C30" s="152">
-        <v>57</v>
-      </c>
-      <c r="D30" s="147">
-        <v>258</v>
-      </c>
-      <c r="E30" s="143">
-        <v>3.8875000000000002</v>
-      </c>
-      <c r="F30" s="152">
-        <v>95</v>
-      </c>
-      <c r="G30" s="147">
-        <v>394</v>
-      </c>
-      <c r="H30" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I30" s="147">
-        <v>0</v>
-      </c>
-      <c r="J30" s="147">
-        <v>0</v>
-      </c>
-      <c r="K30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="151">
-        <v>30</v>
-      </c>
-      <c r="B31" s="143">
-        <v>2.6800000000000001E-2</v>
-      </c>
-      <c r="C31" s="152">
-        <v>29</v>
-      </c>
-      <c r="D31" s="147">
-        <v>141</v>
-      </c>
-      <c r="E31" s="143">
-        <v>1.0582</v>
-      </c>
-      <c r="F31" s="152">
-        <v>95</v>
-      </c>
-      <c r="G31" s="147">
-        <v>394</v>
-      </c>
-      <c r="H31" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I31" s="147">
-        <v>0</v>
-      </c>
-      <c r="J31" s="147">
-        <v>0</v>
-      </c>
-      <c r="K31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="151">
-        <v>31</v>
-      </c>
-      <c r="B32" s="143">
-        <v>0.126</v>
-      </c>
-      <c r="C32" s="152">
-        <v>44</v>
-      </c>
-      <c r="D32" s="147">
-        <v>220</v>
-      </c>
-      <c r="E32" s="143">
-        <v>5.3082000000000003</v>
-      </c>
-      <c r="F32" s="152">
-        <v>44</v>
-      </c>
-      <c r="G32" s="147">
-        <v>220</v>
-      </c>
-      <c r="H32" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I32" s="147">
-        <v>0</v>
-      </c>
-      <c r="J32" s="147">
-        <v>0</v>
-      </c>
-      <c r="K32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="151">
-        <v>32</v>
-      </c>
-      <c r="B33" s="143">
-        <v>0.24690000000000001</v>
-      </c>
-      <c r="C33" s="152">
-        <v>110</v>
-      </c>
-      <c r="D33" s="147">
-        <v>469</v>
-      </c>
-      <c r="E33" s="143">
-        <v>5.5472999999999999</v>
-      </c>
-      <c r="F33" s="152">
-        <v>110</v>
-      </c>
-      <c r="G33" s="147">
-        <v>469</v>
-      </c>
-      <c r="H33" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I33" s="147">
-        <v>0</v>
-      </c>
-      <c r="J33" s="147">
-        <v>0</v>
-      </c>
-      <c r="K33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="151">
-        <v>33</v>
-      </c>
-      <c r="B34" s="143">
-        <v>0.28860000000000002</v>
-      </c>
-      <c r="C34" s="152">
-        <v>87</v>
-      </c>
-      <c r="D34" s="147">
-        <v>389</v>
-      </c>
-      <c r="E34" s="143">
-        <v>3.3715999999999999</v>
-      </c>
-      <c r="F34" s="152">
-        <v>87</v>
-      </c>
-      <c r="G34" s="147">
-        <v>389</v>
-      </c>
-      <c r="H34" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I34" s="147">
-        <v>0</v>
-      </c>
-      <c r="J34" s="147">
-        <v>0</v>
-      </c>
-      <c r="K34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="151">
-        <v>34</v>
-      </c>
-      <c r="B35" s="143">
-        <v>0.22209999999999999</v>
-      </c>
-      <c r="C35" s="152">
-        <v>74</v>
-      </c>
-      <c r="D35" s="147">
-        <v>339</v>
-      </c>
-      <c r="E35" s="143">
-        <v>2.6358999999999999</v>
-      </c>
-      <c r="F35" s="152">
-        <v>74</v>
-      </c>
-      <c r="G35" s="147">
-        <v>339</v>
-      </c>
-      <c r="H35" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I35" s="147">
-        <v>0</v>
-      </c>
-      <c r="J35" s="147">
-        <v>0</v>
-      </c>
-      <c r="K35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="151">
-        <v>35</v>
-      </c>
-      <c r="B36" s="143">
-        <v>0.35149999999999998</v>
-      </c>
-      <c r="C36" s="152">
-        <v>65</v>
-      </c>
-      <c r="D36" s="147">
-        <v>305</v>
-      </c>
-      <c r="E36" s="143">
-        <v>2.1475</v>
-      </c>
-      <c r="F36" s="152">
-        <v>65</v>
-      </c>
-      <c r="G36" s="147">
-        <v>305</v>
-      </c>
-      <c r="H36" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I36" s="147">
-        <v>0</v>
-      </c>
-      <c r="J36" s="147">
-        <v>0</v>
-      </c>
-      <c r="K36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="151">
-        <v>36</v>
-      </c>
-      <c r="B37" s="143">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="C37" s="152">
-        <v>110</v>
-      </c>
-      <c r="D37" s="147">
-        <v>548</v>
-      </c>
-      <c r="E37" s="143">
-        <v>1.4863999999999999</v>
-      </c>
-      <c r="F37" s="152">
-        <v>29</v>
-      </c>
-      <c r="G37" s="147">
-        <v>146</v>
-      </c>
-      <c r="H37" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I37" s="147">
-        <v>0</v>
-      </c>
-      <c r="J37" s="147">
-        <v>0</v>
-      </c>
-      <c r="K37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="151">
-        <v>37</v>
-      </c>
-      <c r="B38" s="143">
-        <v>0.15670000000000001</v>
-      </c>
-      <c r="C38" s="152">
-        <v>113</v>
-      </c>
-      <c r="D38" s="147">
-        <v>564</v>
-      </c>
-      <c r="E38" s="143">
-        <v>8.6432000000000002</v>
-      </c>
-      <c r="F38" s="152">
-        <v>101</v>
-      </c>
-      <c r="G38" s="147">
-        <v>511</v>
-      </c>
-      <c r="H38" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I38" s="147">
-        <v>0</v>
-      </c>
-      <c r="J38" s="147">
-        <v>0</v>
-      </c>
-      <c r="K38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="151">
-        <v>38</v>
-      </c>
-      <c r="B39" s="143">
-        <v>6.0499999999999998E-2</v>
-      </c>
-      <c r="C39" s="152">
-        <v>38</v>
-      </c>
-      <c r="D39" s="147">
-        <v>216</v>
-      </c>
-      <c r="E39" s="143">
-        <v>6.0906000000000002</v>
-      </c>
-      <c r="F39" s="152">
-        <v>76</v>
-      </c>
-      <c r="G39" s="147">
-        <v>402</v>
-      </c>
-      <c r="H39" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I39" s="147">
-        <v>0</v>
-      </c>
-      <c r="J39" s="147">
-        <v>0</v>
-      </c>
-      <c r="K39" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="151">
-        <v>39</v>
-      </c>
-      <c r="B40" s="143">
-        <v>0.13170000000000001</v>
-      </c>
-      <c r="C40" s="152">
-        <v>89</v>
-      </c>
-      <c r="D40" s="147">
-        <v>457</v>
-      </c>
-      <c r="E40" s="143">
-        <v>1.6453</v>
-      </c>
-      <c r="F40" s="152">
-        <v>33</v>
-      </c>
-      <c r="G40" s="147">
-        <v>181</v>
-      </c>
-      <c r="H40" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I40" s="147">
-        <v>0</v>
-      </c>
-      <c r="J40" s="147">
-        <v>0</v>
-      </c>
-      <c r="K40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="151">
-        <v>40</v>
-      </c>
-      <c r="B41" s="143">
-        <v>0.18909999999999999</v>
-      </c>
-      <c r="C41" s="152">
-        <v>118</v>
-      </c>
-      <c r="D41" s="147">
-        <v>582</v>
-      </c>
-      <c r="E41" s="143">
-        <v>1.8115000000000001</v>
-      </c>
-      <c r="F41" s="152">
-        <v>80</v>
-      </c>
-      <c r="G41" s="147">
-        <v>419</v>
-      </c>
-      <c r="H41" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I41" s="147">
-        <v>0</v>
-      </c>
-      <c r="J41" s="147">
-        <v>0</v>
-      </c>
-      <c r="K41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="151">
-        <v>41</v>
-      </c>
-      <c r="B42" s="143">
-        <v>0.22850000000000001</v>
-      </c>
-      <c r="C42" s="152">
-        <v>47</v>
-      </c>
-      <c r="D42" s="147">
-        <v>255</v>
-      </c>
-      <c r="E42" s="143">
-        <v>12.73</v>
-      </c>
-      <c r="F42" s="152">
-        <v>47</v>
-      </c>
-      <c r="G42" s="147">
-        <v>255</v>
-      </c>
-      <c r="H42" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I42" s="147">
-        <v>0</v>
-      </c>
-      <c r="J42" s="147">
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="151">
-        <v>42</v>
-      </c>
-      <c r="B43" s="143">
-        <v>0.34789999999999999</v>
-      </c>
-      <c r="C43" s="152">
-        <v>84</v>
-      </c>
-      <c r="D43" s="147">
-        <v>440</v>
-      </c>
-      <c r="E43" s="143">
-        <v>9.5709</v>
-      </c>
-      <c r="F43" s="152">
-        <v>84</v>
-      </c>
-      <c r="G43" s="147">
-        <v>440</v>
-      </c>
-      <c r="H43" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I43" s="147">
-        <v>0</v>
-      </c>
-      <c r="J43" s="147">
-        <v>0</v>
-      </c>
-      <c r="K43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="151">
-        <v>43</v>
-      </c>
-      <c r="B44" s="143">
-        <v>0.2127</v>
-      </c>
-      <c r="C44" s="152">
-        <v>44</v>
-      </c>
-      <c r="D44" s="147">
-        <v>238</v>
-      </c>
-      <c r="E44" s="143">
-        <v>2.4516</v>
-      </c>
-      <c r="F44" s="152">
-        <v>44</v>
-      </c>
-      <c r="G44" s="147">
-        <v>238</v>
-      </c>
-      <c r="H44" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I44" s="147">
-        <v>0</v>
-      </c>
-      <c r="J44" s="147">
-        <v>0</v>
-      </c>
-      <c r="K44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="151">
-        <v>44</v>
-      </c>
-      <c r="B45" s="143">
-        <v>0.43869999999999998</v>
-      </c>
-      <c r="C45" s="152">
-        <v>92</v>
-      </c>
-      <c r="D45" s="147">
-        <v>481</v>
-      </c>
-      <c r="E45" s="143">
-        <v>8.1262000000000008</v>
-      </c>
-      <c r="F45" s="152">
-        <v>92</v>
-      </c>
-      <c r="G45" s="147">
-        <v>481</v>
-      </c>
-      <c r="H45" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I45" s="147">
-        <v>0</v>
-      </c>
-      <c r="J45" s="147">
-        <v>0</v>
-      </c>
-      <c r="K45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="151">
-        <v>45</v>
-      </c>
-      <c r="B46" s="143">
-        <v>0.35449999999999998</v>
-      </c>
-      <c r="C46" s="152">
-        <v>74</v>
-      </c>
-      <c r="D46" s="147">
-        <v>393</v>
-      </c>
-      <c r="E46" s="143">
-        <v>5.8920000000000003</v>
-      </c>
-      <c r="F46" s="152">
-        <v>74</v>
-      </c>
-      <c r="G46" s="147">
-        <v>393</v>
-      </c>
-      <c r="H46" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I46" s="147">
-        <v>0</v>
-      </c>
-      <c r="J46" s="147">
-        <v>0</v>
-      </c>
-      <c r="K46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="151">
-        <v>46</v>
-      </c>
-      <c r="B47" s="143">
-        <v>0.24030000000000001</v>
-      </c>
-      <c r="C47" s="152">
-        <v>74</v>
-      </c>
-      <c r="D47" s="147">
-        <v>376</v>
-      </c>
-      <c r="E47" s="143">
-        <v>48.258499999999998</v>
-      </c>
-      <c r="F47" s="152">
-        <v>110</v>
-      </c>
-      <c r="G47" s="147">
-        <v>537</v>
-      </c>
-      <c r="H47" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I47" s="147">
-        <v>0</v>
-      </c>
-      <c r="J47" s="147">
-        <v>0</v>
-      </c>
-      <c r="K47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="151">
-        <v>47</v>
-      </c>
-      <c r="B48" s="143">
-        <v>0.18149999999999999</v>
-      </c>
-      <c r="C48" s="152">
-        <v>68</v>
-      </c>
-      <c r="D48" s="147">
-        <v>347</v>
-      </c>
-      <c r="E48" s="143">
-        <v>4.1337000000000002</v>
-      </c>
-      <c r="F48" s="152">
-        <v>36</v>
-      </c>
-      <c r="G48" s="147">
-        <v>198</v>
-      </c>
-      <c r="H48" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I48" s="147">
-        <v>0</v>
-      </c>
-      <c r="J48" s="147">
-        <v>0</v>
-      </c>
-      <c r="K48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="151">
-        <v>48</v>
-      </c>
-      <c r="B49" s="143">
-        <v>0.1797</v>
-      </c>
-      <c r="C49" s="152">
-        <v>57</v>
-      </c>
-      <c r="D49" s="147">
-        <v>300</v>
-      </c>
-      <c r="E49" s="143">
-        <v>2.7877000000000001</v>
-      </c>
-      <c r="F49" s="152">
-        <v>29</v>
-      </c>
-      <c r="G49" s="147">
-        <v>146</v>
-      </c>
-      <c r="H49" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I49" s="147">
-        <v>0</v>
-      </c>
-      <c r="J49" s="147">
-        <v>0</v>
-      </c>
-      <c r="K49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="151">
-        <v>49</v>
-      </c>
-      <c r="B50" s="143">
-        <v>0.27339999999999998</v>
-      </c>
-      <c r="C50" s="152">
-        <v>99</v>
-      </c>
-      <c r="D50" s="147">
-        <v>490</v>
-      </c>
-      <c r="E50" s="143">
-        <v>5.6365999999999996</v>
-      </c>
-      <c r="F50" s="152">
-        <v>44</v>
-      </c>
-      <c r="G50" s="147">
-        <v>239</v>
-      </c>
-      <c r="H50" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I50" s="147">
-        <v>0</v>
-      </c>
-      <c r="J50" s="147">
-        <v>0</v>
-      </c>
-      <c r="K50" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="151">
-        <v>50</v>
-      </c>
-      <c r="B51" s="143">
-        <v>7.4300000000000005E-2</v>
-      </c>
-      <c r="C51" s="152">
-        <v>22</v>
-      </c>
-      <c r="D51" s="147">
-        <v>110</v>
-      </c>
-      <c r="E51" s="143">
-        <v>2.9182999999999999</v>
-      </c>
-      <c r="F51" s="152">
-        <v>65</v>
-      </c>
-      <c r="G51" s="147">
-        <v>336</v>
-      </c>
-      <c r="H51" s="149">
-        <v>-1</v>
-      </c>
-      <c r="I51" s="147">
-        <v>0</v>
-      </c>
-      <c r="J51" s="147">
-        <v>0</v>
-      </c>
-      <c r="K51" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62F289C-7B46-8540-B078-F8A1D05C875C}">
   <dimension ref="B1:E14"/>
   <sheetViews>
@@ -11986,27 +10171,27 @@
       <c r="D12" s="196" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="215">
-        <f>MEDIAN(Sheet1!H2:H11)</f>
-        <v>8.2458500000000008</v>
+      <c r="E12" s="215" t="e">
+        <f>MEDIAN(#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D13" s="196" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="215">
-        <f>MEDIAN(Sheet1!B2:B11)</f>
-        <v>3.6049999999999999E-2</v>
+      <c r="E13" s="215" t="e">
+        <f>MEDIAN(#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D14" s="197" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="216">
-        <f>MEDIAN(Sheet1!E2:E11)</f>
-        <v>0.33550000000000002</v>
+      <c r="E14" s="216" t="e">
+        <f>MEDIAN(#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>